<commit_message>
update final assignments doc
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE44A6-426A-A74E-9C22-9C561280765A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31170E25-05ED-9547-BEF1-746C3EC27F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
@@ -507,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,8 +621,86 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor rgb="FFD5A6BD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -709,13 +787,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -873,6 +975,9 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="7" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -884,32 +989,170 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="7" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="61">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1049,8 +1292,88 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1067,6 +1390,22 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00FF00"/>
           <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1169,8 +1508,32 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1187,6 +1550,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00FF00"/>
           <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1481,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F4DE7E-50A7-8444-BE03-F2EC1C089E28}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView zoomScale="116" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1558,13 +1929,13 @@
       <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="99" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1593,13 +1964,13 @@
       <c r="H3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="99" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1628,13 +1999,13 @@
       <c r="H4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="100" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1663,13 +2034,13 @@
       <c r="H5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="102" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1698,13 +2069,13 @@
       <c r="H6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="103" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1733,13 +2104,13 @@
       <c r="H7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="81" t="s">
         <v>29</v>
       </c>
       <c r="J7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="104" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1768,13 +2139,13 @@
       <c r="H8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="96" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1803,13 +2174,13 @@
       <c r="H9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="95" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1838,13 +2209,13 @@
       <c r="H10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="96" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1873,440 +2244,439 @@
       <c r="H11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="91" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="63" t="s">
-        <v>55</v>
+      <c r="A12" s="66" t="s">
+        <v>74</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F12" s="10">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="G12" s="18">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>58</v>
+      <c r="I12" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="96" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="63" t="s">
-        <v>59</v>
+      <c r="A13" s="66" t="s">
+        <v>77</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F13" s="10">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G13" s="8">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>61</v>
+      <c r="I13" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="96" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="62" t="s">
-        <v>62</v>
+      <c r="A14" s="67" t="s">
+        <v>79</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F14" s="16">
-        <v>0.2</v>
+        <v>0.45</v>
       </c>
       <c r="G14" s="8">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>64</v>
+      <c r="I14" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="93" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="97" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="63" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="F15" s="10">
         <v>0.2</v>
       </c>
       <c r="G15" s="18">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="92" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="96" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="8">
+        <v>25</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="98" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="18">
+        <v>45</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I17" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J17" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="K17" s="103" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F18" s="10">
         <v>0.2</v>
       </c>
-      <c r="G16" s="8">
-        <v>23</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="G17" s="8">
-        <v>38</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="10">
-        <v>0.33</v>
-      </c>
-      <c r="G18" s="18">
+      <c r="G18" s="8">
         <v>40</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>76</v>
+      <c r="I18" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="103" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="66" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="8">
+        <v>42</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="106" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="104" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="G19" s="8">
-        <v>38</v>
-      </c>
-      <c r="H19" s="8" t="s">
+      <c r="E20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="18">
+        <v>21</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="16">
-        <v>0.45</v>
-      </c>
-      <c r="G20" s="8">
-        <v>60</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>76</v>
+      <c r="I20" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="101" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="63" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>41</v>
+        <v>14</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="F21" s="10">
         <v>0.2</v>
       </c>
-      <c r="G21" s="18">
-        <v>36</v>
+      <c r="G21" s="8">
+        <v>23</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="101" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>38</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J22" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="G22" s="8">
-        <v>25</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
+      <c r="K22" s="91" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B22">
-    <cfRule type="endsWith" dxfId="16" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="60" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C22">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="59" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C22">
-    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(C2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="beginsWith" dxfId="12" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="56" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((D2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="55" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E22">
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="54" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2335,26 +2705,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H22">
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(H2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(H2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="48" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
-    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(H2))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I22">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="H1:I11">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:I22 D21:F22 K21:K22 J1:J22">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="1 submission">
+  <conditionalFormatting sqref="J1:J11 D15:E16">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:I22">
+    <cfRule type="containsText" dxfId="45" priority="162" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17:J22">
+    <cfRule type="containsText" dxfId="44" priority="164" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(P12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:I16">
+    <cfRule type="containsText" dxfId="43" priority="166" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:F16 K15:K16 J12:J16 H15:I16">
+    <cfRule type="containsText" dxfId="42" priority="167" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(L18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2363,16 +2751,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74FBE34-1CC7-C24F-8FA9-E46C8B7D73A6}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -2439,13 +2827,13 @@
       <c r="H2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="89" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2474,357 +2862,357 @@
       <c r="H3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="89" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="63" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="10">
+        <v>41</v>
+      </c>
+      <c r="F4" s="55">
         <v>0.2</v>
       </c>
       <c r="G4" s="18">
+        <v>12</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>102</v>
+      <c r="K4" s="88" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="63" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F5" s="10">
         <v>0.2</v>
       </c>
       <c r="G5" s="8">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J5" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="88" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="62" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>88</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="16">
+        <v>41</v>
+      </c>
+      <c r="F6" s="57">
         <v>0.2</v>
       </c>
-      <c r="G6" s="8">
-        <v>17</v>
+      <c r="G6" s="14">
+        <v>10</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="89" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="120" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="113" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="113" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="114" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="115" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="116">
+        <v>0.31</v>
+      </c>
+      <c r="G7" s="114">
+        <v>35</v>
+      </c>
+      <c r="H7" s="114" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="117" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="118" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="119"/>
+    </row>
+    <row r="8" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="107" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>18</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="43"/>
+      <c r="J8" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K8" s="90" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+    <row r="9" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="8">
+        <v>9</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="122">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>17</v>
+      </c>
+      <c r="H10" s="110" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="111" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="120" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="125" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="126" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="127" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="129" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="130">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="131">
+        <v>18</v>
+      </c>
+      <c r="H11" s="132" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="133" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="134" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="135" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="G7" s="18">
-        <v>63</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="8">
-        <v>13</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="48">
-        <v>0.1</v>
-      </c>
-      <c r="G9" s="49">
-        <v>18</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="55">
-        <v>0.31</v>
-      </c>
-      <c r="G10" s="18">
-        <v>35</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="54"/>
-    </row>
-    <row r="11" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="55">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="18">
-        <v>12</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>88</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="G12" s="8">
-        <v>13</v>
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="110">
+        <v>63</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="62" t="s">
-        <v>128</v>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="71" t="s">
+        <v>109</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="57">
-        <v>0.2</v>
-      </c>
-      <c r="G13" s="14">
-        <v>10</v>
+      <c r="F13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="8">
+        <v>13</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="15" t="s">
-        <v>76</v>
-      </c>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="15" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2832,23 +3220,23 @@
     <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="1:11" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:11" s="74" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-    </row>
-    <row r="24" spans="1:11" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:11" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:11" s="69" customFormat="1" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2858,47 +3246,50 @@
     <row r="31" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="32" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="33" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="endsWith" dxfId="31" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="41" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C13">
-    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="40" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="39" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(C2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="beginsWith" dxfId="27" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="37" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((D2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="36" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:E13">
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:E5 J1 D12:E13">
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13">
@@ -2914,30 +3305,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="30" priority="11" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(H2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(H2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="28" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
-    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(H2))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:E12 H1:I1">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="H1:I1 D5:E5">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:E12 D7:E8 J1">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
+  <conditionalFormatting sqref="H4:I7">
+    <cfRule type="containsText" dxfId="26" priority="35" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:I4 F4 K4 J4:J7">
+    <cfRule type="containsText" dxfId="25" priority="36" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(L31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:I13">
+    <cfRule type="containsText" dxfId="24" priority="68" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:J13">
+    <cfRule type="containsText" dxfId="23" priority="70" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(P27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:I3">
+    <cfRule type="containsText" dxfId="22" priority="72" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2 J2:J3">
+    <cfRule type="containsText" dxfId="21" priority="73" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(P22))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2948,14 +3362,34 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:I13">
-    <cfRule type="containsText" dxfId="1" priority="35" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="H11:I11">
+    <cfRule type="containsText" dxfId="20" priority="124" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="containsText" dxfId="19" priority="126" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(P29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:I10">
+    <cfRule type="containsText" dxfId="18" priority="128" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(L24))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2 F11 K11 J2:J13 H11:I11">
-    <cfRule type="containsText" dxfId="0" priority="36" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(L24))))</formula>
+  <conditionalFormatting sqref="J8:J10">
+    <cfRule type="containsText" dxfId="17" priority="130" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(P24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:I7">
+    <cfRule type="containsText" dxfId="16" priority="199" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(L30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="containsText" dxfId="15" priority="201" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(P30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2970,9 +3404,9 @@
   </sheetPr>
   <dimension ref="A1:AF1012"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2991,17 +3425,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="69"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="A1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -4208,15 +4642,15 @@
         <v>88</v>
       </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="71" t="s">
+      <c r="E35" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
     </row>
     <row r="36" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38" t="s">
@@ -4229,15 +4663,15 @@
         <v>88</v>
       </c>
       <c r="D36" s="53"/>
-      <c r="E36" s="71" t="s">
+      <c r="E36" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="70"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
     </row>
     <row r="37" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
@@ -4283,15 +4717,15 @@
         <v>88</v>
       </c>
       <c r="D38" s="52"/>
-      <c r="E38" s="71" t="s">
+      <c r="E38" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
     </row>
     <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -4304,15 +4738,15 @@
         <v>88</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="72" t="s">
+      <c r="E39" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="76"/>
     </row>
     <row r="40" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="63" t="s">
@@ -13166,7 +13600,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{7CE3F55A-FC7F-4646-9491-12CE14B1B5C9}">
+      <autoFilter ref="A2:K42" xr:uid="{D2778026-E447-EE4B-ABDC-E9D2F529333B}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -13183,42 +13617,42 @@
     <mergeCell ref="E39:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="endsWith" dxfId="46" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="14" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C42">
-    <cfRule type="containsText" dxfId="44" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D42">
-    <cfRule type="beginsWith" dxfId="42" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="10" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((D3),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="9" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D3),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E42 G36">
-    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13247,25 +13681,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H37 H40:H42">
-    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H40:H42 H37">
-    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I34 D26:E26 D35 H37:I37 H40:I1012 D41:E41">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I23 D26:F26 H26:I26 D35 H40:I40 D40:E41 J1:J34 D22:F23 K22:K24 K26 D32:E33 J37 F40 K40 J40:J1012">
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update core and pathway
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE0F4EC-E3E0-6F4A-B500-19BB7884AF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002BAE7F-CD31-8943-9597-02CC1BD06B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="500" windowWidth="14080" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="500" windowWidth="21420" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="140">
   <si>
     <t>Course Code</t>
   </si>
@@ -460,12 +460,18 @@
   <si>
     <t>13 OF 21</t>
   </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -539,6 +545,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -918,11 +930,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1356,6 +1369,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1367,17 +1385,44 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="65">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1495,6 +1540,22 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00FFFF"/>
           <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2079,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F4DE7E-50A7-8444-BE03-F2EC1C089E28}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2357,7 +2418,7 @@
       <c r="K7" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="184" t="s">
+      <c r="L7" s="179" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2914,53 +2975,73 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" s="175"/>
+      <c r="G24" s="172" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24">
+        <f>SUM(H2:H22)</f>
+        <v>691</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="G25" s="172" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25">
+        <f>SUM(H24/24)</f>
+        <v>28.791666666666668</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B27" s="185"/>
-      <c r="C27" s="185"/>
+      <c r="A27" s="192">
+        <f>SUM(13 / 21)</f>
+        <v>0.61904761904761907</v>
+      </c>
+      <c r="B27" s="180"/>
+      <c r="C27" s="180"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B28" s="172"/>
-      <c r="C28" s="186"/>
+      <c r="C28" s="181"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C22">
-    <cfRule type="endsWith" dxfId="60" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="64" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((C2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D22">
-    <cfRule type="containsText" dxfId="59" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="63" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="62" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="61" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="beginsWith" dxfId="56" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="60" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((E2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="55" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="59" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((E2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F22">
-    <cfRule type="containsText" dxfId="54" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="58" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="57" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="56" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="55" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2989,43 +3070,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I22">
-    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="54" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="53" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J11">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J16">
-    <cfRule type="containsText" dxfId="46" priority="166" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="50" priority="166" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J16 G15:G16 K12:K16 L15:L16">
-    <cfRule type="containsText" dxfId="45" priority="167" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="49" priority="167" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(M18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:J22">
-    <cfRule type="containsText" dxfId="44" priority="162" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="48" priority="162" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K11 E15:F16">
-    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K22">
-    <cfRule type="containsText" dxfId="42" priority="164" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="46" priority="164" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q12))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3035,10 +3116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74FBE34-1CC7-C24F-8FA9-E46C8B7D73A6}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3450,147 +3531,200 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="177"/>
-    </row>
-    <row r="13" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="177"/>
-      <c r="B13" s="126" t="s">
+    <row r="12" spans="1:12" s="191" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="187"/>
+      <c r="B12" s="188"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="190"/>
+      <c r="H12" s="189"/>
+      <c r="I12" s="189"/>
+      <c r="J12" s="189"/>
+      <c r="K12" s="189"/>
+      <c r="L12" s="188"/>
+    </row>
+    <row r="13" spans="1:12" s="191" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="187"/>
+      <c r="B13" s="188"/>
+      <c r="C13" s="188"/>
+      <c r="D13" s="188"/>
+      <c r="E13" s="189"/>
+      <c r="F13" s="188"/>
+      <c r="G13" s="190"/>
+      <c r="H13" s="189">
+        <f>SUM(H2:H11)</f>
+        <v>172</v>
+      </c>
+      <c r="I13" s="189">
+        <f>SUM(H13/24)</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="J13" s="189"/>
+      <c r="K13" s="189"/>
+      <c r="L13" s="188"/>
+    </row>
+    <row r="14" spans="1:12" s="191" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="187"/>
+      <c r="B14" s="188"/>
+      <c r="C14" s="188"/>
+      <c r="D14" s="188"/>
+      <c r="E14" s="189"/>
+      <c r="F14" s="188"/>
+      <c r="G14" s="190"/>
+      <c r="H14" s="189"/>
+      <c r="I14" s="189"/>
+      <c r="J14" s="189"/>
+      <c r="K14" s="189"/>
+      <c r="L14" s="188"/>
+    </row>
+    <row r="15" spans="1:12" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="177"/>
+    </row>
+    <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="177"/>
+      <c r="B16" s="126" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="96" t="s">
+      <c r="C16" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D16" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="97" t="s">
+      <c r="E16" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="127" t="s">
+      <c r="F16" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="99">
+      <c r="G16" s="99">
         <v>0.1</v>
       </c>
-      <c r="H13" s="97">
+      <c r="H16" s="97">
         <v>63</v>
       </c>
-      <c r="I13" s="97" t="s">
+      <c r="I16" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="100" t="s">
+      <c r="J16" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="101" t="s">
+      <c r="K16" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="128"/>
-    </row>
-    <row r="14" spans="1:12" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="177"/>
-      <c r="B14" s="129" t="s">
+      <c r="L16" s="128"/>
+    </row>
+    <row r="17" spans="1:12" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="177"/>
+      <c r="B17" s="129" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C17" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="108" t="s">
+      <c r="D17" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="109" t="s">
+      <c r="E17" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="130" t="s">
+      <c r="F17" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="109" t="s">
+      <c r="G17" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="109">
+      <c r="H17" s="109">
         <v>13</v>
       </c>
-      <c r="I14" s="109" t="s">
+      <c r="I17" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="112" t="s">
+      <c r="J17" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="113" t="s">
+      <c r="K17" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="131"/>
-    </row>
-    <row r="15" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="172" t="s">
+      <c r="L17" s="131"/>
+    </row>
+    <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="172" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="193">
+        <f>SUM(2 / 9)</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="33" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C14">
-    <cfRule type="endsWith" dxfId="41" priority="10" operator="endsWith" text="*">
+  <conditionalFormatting sqref="C2:C17">
+    <cfRule type="endsWith" dxfId="45" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((C2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D14">
-    <cfRule type="containsText" dxfId="40" priority="15" operator="containsText" text="Elective">
+  <conditionalFormatting sqref="D1:D17">
+    <cfRule type="containsText" dxfId="44" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D14">
-    <cfRule type="containsText" dxfId="39" priority="8" operator="containsText" text="pathway">
+  <conditionalFormatting sqref="D2:D17">
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
-    <cfRule type="beginsWith" dxfId="37" priority="16" operator="beginsWith" text="R">
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="beginsWith" dxfId="41" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((E2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="40" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((E2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:F14">
-    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="Essay">
+  <conditionalFormatting sqref="E2:F17">
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:F5 K1 E13:F14">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="1 submission">
+  <conditionalFormatting sqref="E4:F5 K1 E16:F17">
+    <cfRule type="containsText" dxfId="35" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
@@ -3602,7 +3736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="9"/>
@@ -3614,80 +3748,100 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
-    <cfRule type="containsText" dxfId="30" priority="11" operator="containsText" text="A">
+  <conditionalFormatting sqref="I2:I17">
+    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1 E5:F5">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J3">
-    <cfRule type="containsText" dxfId="26" priority="72" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(M22))))</formula>
+    <cfRule type="containsText" dxfId="30" priority="72" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4 G4 L4 K4:K7">
-    <cfRule type="containsText" dxfId="25" priority="36" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(M31))))</formula>
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J7">
-    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(M31))))</formula>
+    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:J7">
-    <cfRule type="containsText" dxfId="23" priority="199" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="199" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:J10">
+    <cfRule type="containsText" dxfId="26" priority="128" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:J15">
+    <cfRule type="containsText" dxfId="25" priority="124" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:J17">
+    <cfRule type="containsText" dxfId="24" priority="68" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M30))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:J10">
-    <cfRule type="containsText" dxfId="22" priority="128" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(M24))))</formula>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="23" priority="201" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:J12">
-    <cfRule type="containsText" dxfId="21" priority="124" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(M29))))</formula>
+  <conditionalFormatting sqref="K8:K10">
+    <cfRule type="containsText" dxfId="22" priority="130" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q27))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:J14">
-    <cfRule type="containsText" dxfId="20" priority="68" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(M27))))</formula>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="21" priority="126" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="19" priority="201" operator="containsText" text="1 submission">
+  <conditionalFormatting sqref="K16:K17">
+    <cfRule type="containsText" dxfId="20" priority="70" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q30))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10">
-    <cfRule type="containsText" dxfId="18" priority="130" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q24))))</formula>
+  <conditionalFormatting sqref="L2 K2:K3">
+    <cfRule type="containsText" dxfId="19" priority="73" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q25))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K12">
-    <cfRule type="containsText" dxfId="17" priority="126" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q29))))</formula>
+  <conditionalFormatting sqref="I14:J14">
+    <cfRule type="containsText" dxfId="18" priority="205" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:K14">
-    <cfRule type="containsText" dxfId="16" priority="70" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q27))))</formula>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsText" dxfId="17" priority="207" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q34))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2 K2:K3">
-    <cfRule type="containsText" dxfId="15" priority="73" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q22))))</formula>
+  <conditionalFormatting sqref="I11:J13">
+    <cfRule type="containsText" dxfId="1" priority="212" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(M32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11:K13">
+    <cfRule type="containsText" dxfId="0" priority="214" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3723,17 +3877,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="179"/>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
+      <c r="A1" s="182"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
+      <c r="F1" s="183"/>
+      <c r="G1" s="183"/>
+      <c r="H1" s="183"/>
+      <c r="I1" s="183"/>
+      <c r="J1" s="183"/>
+      <c r="K1" s="183"/>
     </row>
     <row r="2" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -4940,15 +5094,15 @@
         <v>88</v>
       </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="181" t="s">
+      <c r="E35" s="184" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="180"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="180"/>
-      <c r="J35" s="180"/>
-      <c r="K35" s="180"/>
+      <c r="F35" s="183"/>
+      <c r="G35" s="183"/>
+      <c r="H35" s="183"/>
+      <c r="I35" s="183"/>
+      <c r="J35" s="183"/>
+      <c r="K35" s="183"/>
     </row>
     <row r="36" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38" t="s">
@@ -4961,15 +5115,15 @@
         <v>88</v>
       </c>
       <c r="D36" s="53"/>
-      <c r="E36" s="181" t="s">
+      <c r="E36" s="184" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="180"/>
-      <c r="G36" s="180"/>
-      <c r="H36" s="180"/>
-      <c r="I36" s="180"/>
-      <c r="J36" s="180"/>
-      <c r="K36" s="180"/>
+      <c r="F36" s="183"/>
+      <c r="G36" s="183"/>
+      <c r="H36" s="183"/>
+      <c r="I36" s="183"/>
+      <c r="J36" s="183"/>
+      <c r="K36" s="183"/>
     </row>
     <row r="37" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
@@ -5015,15 +5169,15 @@
         <v>88</v>
       </c>
       <c r="D38" s="52"/>
-      <c r="E38" s="181" t="s">
+      <c r="E38" s="184" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="180"/>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="180"/>
-      <c r="J38" s="180"/>
-      <c r="K38" s="180"/>
+      <c r="F38" s="183"/>
+      <c r="G38" s="183"/>
+      <c r="H38" s="183"/>
+      <c r="I38" s="183"/>
+      <c r="J38" s="183"/>
+      <c r="K38" s="183"/>
     </row>
     <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -5036,15 +5190,15 @@
         <v>88</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="182" t="s">
+      <c r="E39" s="185" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="183"/>
-      <c r="G39" s="183"/>
-      <c r="H39" s="183"/>
-      <c r="I39" s="183"/>
-      <c r="J39" s="183"/>
-      <c r="K39" s="183"/>
+      <c r="F39" s="186"/>
+      <c r="G39" s="186"/>
+      <c r="H39" s="186"/>
+      <c r="I39" s="186"/>
+      <c r="J39" s="186"/>
+      <c r="K39" s="186"/>
     </row>
     <row r="40" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="63" t="s">
@@ -13898,7 +14052,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{7A84D793-EE89-1140-86F9-2FC4A6230973}">
+      <autoFilter ref="A2:K42" xr:uid="{A5D84C3A-31D1-5942-85BD-3D0C27AC719C}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -13915,42 +14069,42 @@
     <mergeCell ref="E39:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="endsWith" dxfId="14" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="16" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C42">
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D42">
-    <cfRule type="beginsWith" dxfId="10" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="12" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((D3),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="11" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D3),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E42 G36">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13979,25 +14133,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H37 H40:H42">
-    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H40:H42 H37">
-    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I34 D26:E26 D35 H37:I37 H40:I1012 D41:E41">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I23 D26:F26 H26:I26 D35 H40:I40 D40:E41 J1:J34 D22:F23 K22:K24 K26 D32:E33 J37 F40 K40 J40:J1012">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update data mining project pdfs
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5E67B5-ABD1-854A-B278-A4AD92FDC6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D7EF7-0BFC-3E4D-94BF-C6D098BF3BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="500" windowWidth="20720" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12880" yWindow="500" windowWidth="20720" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="170">
   <si>
     <t>Course Code</t>
   </si>
@@ -550,6 +550,12 @@
   </si>
   <si>
     <t>3 OF 9</t>
+  </si>
+  <si>
+    <t>Grades</t>
+  </si>
+  <si>
+    <t>Core/Elective</t>
   </si>
 </sst>
 </file>
@@ -1501,6 +1507,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1512,9 +1521,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -3327,7 +3333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74FBE34-1CC7-C24F-8FA9-E46C8B7D73A6}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -3457,7 +3463,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="195" t="s">
+      <c r="A4" s="190" t="s">
         <v>133</v>
       </c>
       <c r="B4" s="95" t="s">
@@ -4088,17 +4094,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="190"/>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
+      <c r="A1" s="191"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
     </row>
     <row r="2" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -5305,15 +5311,15 @@
         <v>88</v>
       </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="192" t="s">
+      <c r="E35" s="193" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="191"/>
-      <c r="G35" s="191"/>
-      <c r="H35" s="191"/>
-      <c r="I35" s="191"/>
-      <c r="J35" s="191"/>
-      <c r="K35" s="191"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
+      <c r="K35" s="192"/>
     </row>
     <row r="36" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38" t="s">
@@ -5326,15 +5332,15 @@
         <v>88</v>
       </c>
       <c r="D36" s="53"/>
-      <c r="E36" s="192" t="s">
+      <c r="E36" s="193" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="191"/>
-      <c r="G36" s="191"/>
-      <c r="H36" s="191"/>
-      <c r="I36" s="191"/>
-      <c r="J36" s="191"/>
-      <c r="K36" s="191"/>
+      <c r="F36" s="192"/>
+      <c r="G36" s="192"/>
+      <c r="H36" s="192"/>
+      <c r="I36" s="192"/>
+      <c r="J36" s="192"/>
+      <c r="K36" s="192"/>
     </row>
     <row r="37" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
@@ -5380,15 +5386,15 @@
         <v>88</v>
       </c>
       <c r="D38" s="52"/>
-      <c r="E38" s="192" t="s">
+      <c r="E38" s="193" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="191"/>
-      <c r="G38" s="191"/>
-      <c r="H38" s="191"/>
-      <c r="I38" s="191"/>
-      <c r="J38" s="191"/>
-      <c r="K38" s="191"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
+      <c r="H38" s="192"/>
+      <c r="I38" s="192"/>
+      <c r="J38" s="192"/>
+      <c r="K38" s="192"/>
     </row>
     <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -5401,15 +5407,15 @@
         <v>88</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="193" t="s">
+      <c r="E39" s="194" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="194"/>
-      <c r="G39" s="194"/>
-      <c r="H39" s="194"/>
-      <c r="I39" s="194"/>
-      <c r="J39" s="194"/>
-      <c r="K39" s="194"/>
+      <c r="F39" s="195"/>
+      <c r="G39" s="195"/>
+      <c r="H39" s="195"/>
+      <c r="I39" s="195"/>
+      <c r="J39" s="195"/>
+      <c r="K39" s="195"/>
     </row>
     <row r="40" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="63" t="s">
@@ -14263,7 +14269,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{723ACAC7-DE43-8B44-B9A3-A0C190CE3930}">
+      <autoFilter ref="A2:K42" xr:uid="{957E98E7-215B-AD4A-98D2-35235256C3DC}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -14374,475 +14380,487 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B9180E-E31E-2D47-9384-8D5049DEA67E}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="185" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="185" customWidth="1"/>
-    <col min="3" max="3" width="70" style="185" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="185" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="10.83203125" style="185"/>
-    <col min="9" max="9" width="13.5" style="185" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="185"/>
+    <col min="1" max="2" width="20.33203125" style="185" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="185" customWidth="1"/>
+    <col min="4" max="4" width="70" style="185" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" style="185" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="185"/>
+    <col min="7" max="7" width="6.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="185" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="185" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="185"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="185" t="s">
         <v>142</v>
       </c>
+      <c r="B1" s="185" t="s">
+        <v>168</v>
+      </c>
       <c r="F1" s="185" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="185" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="185" t="s">
+      <c r="I1" s="185" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="185" t="s">
         <v>141</v>
       </c>
       <c r="B3" s="185" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="185" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="186" t="s">
+      <c r="D3" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="185" t="s">
+      <c r="F3" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="185" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="185" t="s">
+      <c r="C5" s="185" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="186" t="s">
+      <c r="D5" s="186" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="185" t="s">
+      <c r="F5" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="185">
+      <c r="G5" s="185">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="185" t="s">
+    <row r="6" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="186" t="s">
+      <c r="D6" s="186" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="185" t="s">
+      <c r="F6" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="185">
+      <c r="G6" s="185">
         <v>38</v>
       </c>
-      <c r="G6" s="185">
-        <f>SUM(F5+F6)</f>
+      <c r="H6" s="185">
+        <f>SUM(G5+G6)</f>
         <v>72</v>
       </c>
-      <c r="H6" s="185">
+      <c r="I6" s="185">
         <v>53</v>
       </c>
-      <c r="I6" s="189">
+      <c r="J6" s="189">
         <f>SUM(72/53)</f>
         <v>1.3584905660377358</v>
       </c>
-      <c r="J6" s="185" t="s">
+      <c r="K6" s="185" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="185" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="185" t="s">
+      <c r="C8" s="185" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="186" t="s">
+      <c r="D8" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="185" t="s">
+      <c r="E8" s="185" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="185" t="s">
+      <c r="F8" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="185" t="s">
+    <row r="9" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="185" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="186" t="s">
+      <c r="D9" s="186" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="185" t="s">
+      <c r="F9" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="185" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="185" t="s">
+      <c r="C11" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="186" t="s">
+      <c r="D11" s="186" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="185" t="s">
+      <c r="E11" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="185" t="s">
+      <c r="F11" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="185" t="s">
+    <row r="12" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="185" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="186" t="s">
+      <c r="D12" s="186" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="185" t="s">
+      <c r="F12" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="185" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="185" t="s">
+      <c r="C14" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="186" t="s">
+      <c r="D14" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="185" t="s">
+      <c r="E14" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="E14" s="185" t="s">
+      <c r="F14" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="185" t="s">
+    <row r="15" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="186" t="s">
+      <c r="D15" s="186" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="185" t="s">
+      <c r="E15" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="185" t="s">
+      <c r="F15" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="185" t="s">
+    <row r="16" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="186" t="s">
+      <c r="D16" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="185" t="s">
+      <c r="F16" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="185" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="185" t="s">
+      <c r="C18" s="185" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="186" t="s">
+      <c r="D18" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="185" t="s">
+      <c r="E18" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="E18" s="185" t="s">
+      <c r="F18" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="185" t="s">
+    <row r="19" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="185" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="186" t="s">
+      <c r="D19" s="186" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="185" t="s">
+      <c r="F19" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="185" t="s">
+    <row r="20" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="186" t="s">
+      <c r="D20" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="185" t="s">
+      <c r="F20" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="185" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="185" t="s">
+      <c r="C22" s="185" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="186" t="s">
+      <c r="D22" s="186" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="185" t="s">
+      <c r="F22" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="185" t="s">
+    <row r="23" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="186" t="s">
+      <c r="D23" s="186" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="185" t="s">
+      <c r="F23" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="185" t="s">
+    <row r="24" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="186" t="s">
+      <c r="D24" s="186" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="185" t="s">
+      <c r="F24" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="185" t="s">
         <v>149</v>
       </c>
-      <c r="B26" s="188" t="s">
+      <c r="C26" s="188" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="186" t="s">
+      <c r="D26" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="185" t="s">
+      <c r="F26" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="187" t="s">
+    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="187" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="186" t="s">
+      <c r="D27" s="186" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="185" t="s">
+      <c r="F27" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="187" t="s">
+    <row r="28" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="187" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="186" t="s">
+      <c r="D28" s="186" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="185" t="s">
+      <c r="F28" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="185" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="185" t="s">
+      <c r="C30" s="185" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="186" t="s">
+      <c r="D30" s="186" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="185" t="s">
+      <c r="F30" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="185" t="s">
+    <row r="31" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="185" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="186" t="s">
+      <c r="D31" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="185" t="s">
+      <c r="F31" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="185" t="s">
+    <row r="32" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="186" t="s">
+      <c r="D32" s="186" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="185" t="s">
+      <c r="F32" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="185" t="s">
         <v>151</v>
       </c>
-      <c r="B34" s="185" t="s">
+      <c r="C34" s="185" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="186" t="s">
+      <c r="D34" s="186" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="185" t="s">
+      <c r="F34" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="185" t="s">
+    <row r="35" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="185" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="187" t="s">
+      <c r="D35" s="187" t="s">
         <v>125</v>
       </c>
-      <c r="E35" s="185" t="s">
+      <c r="F35" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="185" t="s">
+    <row r="36" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="185" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="187" t="s">
+      <c r="D36" s="187" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="185" t="s">
+      <c r="F36" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="185" t="s">
+    <row r="37" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="185" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="187" t="s">
+      <c r="D37" s="187" t="s">
         <v>129</v>
       </c>
-      <c r="E37" s="185" t="s">
+      <c r="F37" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="185" t="s">
         <v>152</v>
       </c>
-      <c r="B39" s="185" t="s">
+      <c r="C39" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="187" t="s">
+      <c r="D39" s="187" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="185" t="s">
+      <c r="F39" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="185" t="s">
+    <row r="40" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="185" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="187" t="s">
+      <c r="D40" s="187" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="185" t="s">
+      <c r="F40" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="185" t="s">
+    <row r="41" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="185" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="185" t="s">
+    <row r="42" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="185" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
-  <conditionalFormatting sqref="C3 C5:C6">
+  <conditionalFormatting sqref="D3 D5:D6">
     <cfRule type="endsWith" dxfId="9" priority="15" operator="endsWith" text="*">
-      <formula>RIGHT((C3),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C9">
+  <conditionalFormatting sqref="D8:D9">
     <cfRule type="endsWith" dxfId="8" priority="13" operator="endsWith" text="*">
-      <formula>RIGHT((C8),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D8),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
+  <conditionalFormatting sqref="D11:D12">
     <cfRule type="endsWith" dxfId="7" priority="11" operator="endsWith" text="*">
-      <formula>RIGHT((C11),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D11),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C16">
+  <conditionalFormatting sqref="D14:D16">
     <cfRule type="endsWith" dxfId="6" priority="9" operator="endsWith" text="*">
-      <formula>RIGHT((C14),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D14),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C20">
+  <conditionalFormatting sqref="D18:D20">
     <cfRule type="endsWith" dxfId="5" priority="8" operator="endsWith" text="*">
-      <formula>RIGHT((C18),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D18),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C24">
+  <conditionalFormatting sqref="D22:D24">
     <cfRule type="endsWith" dxfId="4" priority="7" operator="endsWith" text="*">
-      <formula>RIGHT((C22),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D22),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C28">
+  <conditionalFormatting sqref="D26:D28">
     <cfRule type="endsWith" dxfId="3" priority="5" operator="endsWith" text="*">
-      <formula>RIGHT((C26),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D26),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C32">
+  <conditionalFormatting sqref="D30:D32">
     <cfRule type="endsWith" dxfId="2" priority="6" operator="endsWith" text="*">
-      <formula>RIGHT((C30),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D30),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C37">
+  <conditionalFormatting sqref="D34:D37">
     <cfRule type="endsWith" dxfId="1" priority="3" operator="endsWith" text="*">
-      <formula>RIGHT((C34),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D34),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:C40">
+  <conditionalFormatting sqref="D39:D40">
     <cfRule type="endsWith" dxfId="0" priority="1" operator="endsWith" text="*">
-      <formula>RIGHT((C39),LEN("*"))=("*")</formula>
+      <formula>RIGHT((D39),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update data mining project
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D7EF7-0BFC-3E4D-94BF-C6D098BF3BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8093EB7-FF9D-A047-893E-C4DCBBC552B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="500" windowWidth="20720" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12880" yWindow="500" windowWidth="20720" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="176">
   <si>
     <t>Course Code</t>
   </si>
@@ -556,6 +556,24 @@
   </si>
   <si>
     <t>Core/Elective</t>
+  </si>
+  <si>
+    <t>Projj</t>
+  </si>
+  <si>
+    <t>proj</t>
+  </si>
+  <si>
+    <t>essay</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>Proj</t>
+  </si>
+  <si>
+    <t>exam</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1072,7 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1521,13 +1539,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="76">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1635,16 +1662,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1659,8 +1686,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1675,8 +1702,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1691,8 +1726,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1701,14 +1736,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFEA9999"/>
           <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1867,8 +1894,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1883,8 +1910,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1899,8 +1926,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFD5A6BD"/>
           <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1915,16 +1958,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1939,8 +1974,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1949,14 +1984,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFEA9999"/>
           <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2027,8 +2054,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2043,8 +2070,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2059,8 +2094,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2075,8 +2110,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2085,14 +2120,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFCFE2F3"/>
           <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2342,7 +2369,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3221,43 +3248,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="endsWith" dxfId="74" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="75" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((D2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E22">
-    <cfRule type="containsText" dxfId="73" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="74" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="containsText" dxfId="72" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="73" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="72" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
+    <cfRule type="beginsWith" dxfId="71" priority="16" operator="beginsWith" text="R">
+      <formula>LEFT((F2),LEN("R"))=("R")</formula>
+    </cfRule>
     <cfRule type="beginsWith" dxfId="70" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((F2),LEN("Python"))=("Python")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="69" priority="16" operator="beginsWith" text="R">
-      <formula>LEFT((F2),LEN("R"))=("R")</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G22">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(F2))))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="3" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(F2))))</formula>
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="Exam">
+      <formula>NOT(ISERROR(SEARCH(("Exam"),(F2))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(F2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="Exam">
-      <formula>NOT(ISERROR(SEARCH(("Exam"),(F2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H22">
@@ -3285,43 +3312,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J22">
-    <cfRule type="containsText" dxfId="64" priority="13" operator="containsText" text="I">
-      <formula>NOT(ISERROR(SEARCH(("I"),(J2))))</formula>
+    <cfRule type="containsText" dxfId="65" priority="11" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="64" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="11" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(J2))))</formula>
+    <cfRule type="containsText" dxfId="63" priority="13" operator="containsText" text="I">
+      <formula>NOT(ISERROR(SEARCH(("I"),(J2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K11">
-    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:K16">
-    <cfRule type="containsText" dxfId="60" priority="166" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="166" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:K16 H15:H16 L12:L16 M15:M16">
-    <cfRule type="containsText" dxfId="59" priority="167" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="60" priority="167" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:K22">
-    <cfRule type="containsText" dxfId="58" priority="162" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="59" priority="162" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L11 F15:G16">
-    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L22">
-    <cfRule type="containsText" dxfId="56" priority="164" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="57" priority="164" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(R12))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3897,47 +3924,47 @@
     <row r="36" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="endsWith" dxfId="55" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="56" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((C2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D17">
-    <cfRule type="containsText" dxfId="54" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="55" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
+    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="pathway">
+      <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="53" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="pathway">
-      <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
+    <cfRule type="beginsWith" dxfId="52" priority="16" operator="beginsWith" text="R">
+      <formula>LEFT((E2),LEN("R"))=("R")</formula>
+    </cfRule>
     <cfRule type="beginsWith" dxfId="51" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((E2),LEN("Python"))=("Python")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="16" operator="beginsWith" text="R">
-      <formula>LEFT((E2),LEN("R"))=("R")</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F17">
-    <cfRule type="containsText" dxfId="49" priority="6" operator="containsText" text="Programming">
-      <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
+    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
+    <cfRule type="containsText" dxfId="48" priority="5" operator="containsText" text="Exam">
+      <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="5" operator="containsText" text="Exam">
-      <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
+    <cfRule type="containsText" dxfId="47" priority="6" operator="containsText" text="Programming">
+      <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F5 K1 E16:F17">
-    <cfRule type="containsText" dxfId="45" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3966,98 +3993,98 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="I">
-      <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
+    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="44" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="11" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
+    <cfRule type="containsText" dxfId="43" priority="13" operator="containsText" text="I">
+      <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1 E5:F5">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J3">
-    <cfRule type="containsText" dxfId="40" priority="72" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="72" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4 G4 L4 K4:K7">
-    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J7">
-    <cfRule type="containsText" dxfId="38" priority="35" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="35" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:J7">
-    <cfRule type="containsText" dxfId="37" priority="199" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="199" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J10">
-    <cfRule type="containsText" dxfId="36" priority="128" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="128" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:J13">
-    <cfRule type="containsText" dxfId="35" priority="212" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="212" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J14">
-    <cfRule type="containsText" dxfId="34" priority="205" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="205" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J15">
-    <cfRule type="containsText" dxfId="33" priority="124" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="124" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:J17">
-    <cfRule type="containsText" dxfId="32" priority="68" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="68" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="31" priority="201" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="32" priority="201" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K10">
-    <cfRule type="containsText" dxfId="30" priority="130" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="31" priority="130" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K13">
-    <cfRule type="containsText" dxfId="29" priority="214" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="30" priority="214" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="28" priority="207" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="29" priority="207" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="27" priority="126" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="28" priority="126" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K17">
-    <cfRule type="containsText" dxfId="26" priority="70" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="27" priority="70" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2 K2:K3">
-    <cfRule type="containsText" dxfId="25" priority="73" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="26" priority="73" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q25))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4073,9 +4100,9 @@
   </sheetPr>
   <dimension ref="A1:AF1012"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3:I5"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14269,7 +14296,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{957E98E7-215B-AD4A-98D2-35235256C3DC}">
+      <autoFilter ref="A2:K42" xr:uid="{8C91CB1A-E796-3343-9804-0D08AA5DE123}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -14286,42 +14313,42 @@
     <mergeCell ref="E39:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="endsWith" dxfId="24" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="25" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C42">
+    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="pathway">
+      <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="pathway">
-      <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D42">
+    <cfRule type="beginsWith" dxfId="21" priority="16" operator="beginsWith" text="R">
+      <formula>LEFT((D3),LEN("R"))=("R")</formula>
+    </cfRule>
     <cfRule type="beginsWith" dxfId="20" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D3),LEN("Python"))=("Python")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="16" operator="beginsWith" text="R">
-      <formula>LEFT((D3),LEN("R"))=("R")</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E42 G36">
-    <cfRule type="containsText" dxfId="18" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="Project">
+      <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Project">
-      <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14350,25 +14377,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H37 H40:H42">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="B">
-      <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H40:H42 H37">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I34 D26:E26 D35 H37:I37 H40:I1012 D41:E41">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I23 D26:F26 H26:I26 D35 H40:I40 D40:E41 J1:J34 D22:F23 K22:K24 K26 D32:E33 J37 F40 K40 J40:J1012">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14380,487 +14407,639 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B9180E-E31E-2D47-9384-8D5049DEA67E}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.33203125" style="185" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="185" customWidth="1"/>
-    <col min="4" max="4" width="70" style="185" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" style="185" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="185"/>
-    <col min="7" max="7" width="6.33203125" style="185" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="185" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="185" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="185" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="185"/>
+    <col min="1" max="1" width="20.33203125" style="185" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="196" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="185" customWidth="1"/>
+    <col min="5" max="5" width="70" style="185" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="185" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="185"/>
+    <col min="8" max="8" width="6.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="185" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="185" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="185"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="185" t="s">
         <v>142</v>
       </c>
       <c r="B1" s="185" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="185" t="s">
+      <c r="C1" s="196" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="185" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="185" t="s">
+      <c r="H1" s="185" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="185" t="s">
+      <c r="J1" s="185" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="185" t="s">
         <v>141</v>
       </c>
       <c r="B3" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="185" t="s">
+      <c r="D3" s="185" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="186" t="s">
+      <c r="E3" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="185" t="s">
+      <c r="G3" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="185" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="185" t="s">
+      <c r="B5" s="185" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="185" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="186" t="s">
+      <c r="E5" s="186" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="185" t="s">
+      <c r="G5" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="185">
+      <c r="H5" s="185">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="185" t="s">
+    <row r="6" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="185" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="185" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="186" t="s">
+      <c r="E6" s="186" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="185" t="s">
+      <c r="G6" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="185">
+      <c r="H6" s="185">
         <v>38</v>
       </c>
-      <c r="H6" s="185">
-        <f>SUM(G5+G6)</f>
+      <c r="I6" s="185">
+        <f>SUM(H5+H6)</f>
         <v>72</v>
       </c>
-      <c r="I6" s="185">
+      <c r="J6" s="185">
         <v>53</v>
       </c>
-      <c r="J6" s="189">
+      <c r="K6" s="189">
         <f>SUM(72/53)</f>
         <v>1.3584905660377358</v>
       </c>
-      <c r="K6" s="185" t="s">
+      <c r="L6" s="185" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="185" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="B8" s="185" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="196">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="185" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="186" t="s">
+      <c r="E8" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="185" t="s">
+      <c r="F8" s="185" t="s">
         <v>153</v>
       </c>
-      <c r="F8" s="185" t="s">
+      <c r="G8" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="185" t="s">
+    <row r="9" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="185" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="196">
+        <v>0.35</v>
+      </c>
+      <c r="D9" s="185" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="186" t="s">
+      <c r="E9" s="186" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="185" t="s">
+      <c r="G9" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="185" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="185" t="s">
+      <c r="B11" s="185" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="196">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D11" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="186" t="s">
+      <c r="E11" s="186" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="185" t="s">
+      <c r="F11" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="F11" s="185" t="s">
+      <c r="G11" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="185" t="s">
+    <row r="12" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="185" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="196">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="185" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="186" t="s">
+      <c r="E12" s="186" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="185" t="s">
+      <c r="G12" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="185" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="185" t="s">
+      <c r="B14" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="196">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="186" t="s">
+      <c r="E14" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="185" t="s">
+      <c r="F14" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="F14" s="185" t="s">
+      <c r="G14" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="185" t="s">
+    <row r="15" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="196">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="186" t="s">
+      <c r="E15" s="186" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="185" t="s">
+      <c r="F15" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="185" t="s">
+      <c r="G15" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="185" t="s">
+    <row r="16" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="196">
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="186" t="s">
+      <c r="E16" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="185" t="s">
+      <c r="G16" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="185" t="s">
         <v>146</v>
       </c>
-      <c r="C18" s="185" t="s">
+      <c r="B18" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="196">
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="185" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="186" t="s">
+      <c r="E18" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="185" t="s">
+      <c r="F18" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="185" t="s">
+      <c r="G18" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="185" t="s">
+    <row r="19" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="196">
+        <v>0.2</v>
+      </c>
+      <c r="D19" s="185" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="186" t="s">
+      <c r="E19" s="186" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="185" t="s">
+      <c r="G19" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="185" t="s">
+    <row r="20" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="196">
+        <v>0.22</v>
+      </c>
+      <c r="D20" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="186" t="s">
+      <c r="E20" s="186" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="185" t="s">
+      <c r="G20" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="185" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="185" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="185" t="s">
+      <c r="B22" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="185" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="186" t="s">
+      <c r="E22" s="186" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="185" t="s">
+      <c r="G22" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="185" t="s">
+    <row r="23" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="186" t="s">
+      <c r="E23" s="186" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="185" t="s">
+      <c r="G23" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="185" t="s">
+    <row r="24" spans="1:7" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="186" t="s">
+      <c r="E24" s="186" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="185" t="s">
+      <c r="G24" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="185" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="188" t="s">
+      <c r="B26" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="188" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="186" t="s">
+      <c r="E26" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="185" t="s">
+      <c r="G26" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="187" t="s">
+    <row r="27" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="187" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="186" t="s">
+      <c r="E27" s="186" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="185" t="s">
+      <c r="G27" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="187" t="s">
+    <row r="28" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="185" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="187" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="186" t="s">
+      <c r="E28" s="186" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="185" t="s">
+      <c r="G28" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="185" t="s">
         <v>150</v>
       </c>
-      <c r="C30" s="185" t="s">
+      <c r="B30" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="185" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="186" t="s">
+      <c r="E30" s="186" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="185" t="s">
+      <c r="G30" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="185" t="s">
+    <row r="31" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="185" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="186" t="s">
+      <c r="E31" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="185" t="s">
+      <c r="G31" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="185" t="s">
+    <row r="32" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="185" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="186" t="s">
+      <c r="E32" s="186" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="185" t="s">
+      <c r="G32" s="185" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="185" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="185" t="s">
+      <c r="B34" s="185" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="185" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="186" t="s">
+      <c r="E34" s="186" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="185" t="s">
+      <c r="G34" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="185" t="s">
+    <row r="35" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="D35" s="185" t="s">
         <v>124</v>
       </c>
-      <c r="D35" s="187" t="s">
+      <c r="E35" s="187" t="s">
         <v>125</v>
       </c>
-      <c r="F35" s="185" t="s">
+      <c r="G35" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="185" t="s">
+    <row r="36" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="185" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="187" t="s">
+      <c r="E36" s="187" t="s">
         <v>127</v>
       </c>
-      <c r="F36" s="185" t="s">
+      <c r="G36" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="185" t="s">
+    <row r="37" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="185" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="185" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="187" t="s">
+      <c r="E37" s="187" t="s">
         <v>129</v>
       </c>
-      <c r="F37" s="185" t="s">
+      <c r="G37" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="185" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="185" t="s">
+      <c r="B39" s="185" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="187" t="s">
+      <c r="E39" s="187" t="s">
         <v>119</v>
       </c>
-      <c r="F39" s="185" t="s">
+      <c r="G39" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="185" t="s">
+    <row r="40" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="185" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="187" t="s">
+      <c r="E40" s="187" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="185" t="s">
+      <c r="G40" s="185" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="185" t="s">
+    <row r="41" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D41" s="185" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="185" t="s">
+    <row r="42" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D42" s="185" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
-  <conditionalFormatting sqref="D3 D5:D6">
-    <cfRule type="endsWith" dxfId="9" priority="15" operator="endsWith" text="*">
-      <formula>RIGHT((D3),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E3 E5:E6">
+    <cfRule type="endsWith" dxfId="10" priority="18" operator="endsWith" text="*">
+      <formula>RIGHT((E3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
-    <cfRule type="endsWith" dxfId="8" priority="13" operator="endsWith" text="*">
-      <formula>RIGHT((D8),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E8:E9">
+    <cfRule type="endsWith" dxfId="9" priority="16" operator="endsWith" text="*">
+      <formula>RIGHT((E8),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="endsWith" dxfId="7" priority="11" operator="endsWith" text="*">
-      <formula>RIGHT((D11),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E11:E12">
+    <cfRule type="endsWith" dxfId="8" priority="14" operator="endsWith" text="*">
+      <formula>RIGHT((E11),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D16">
-    <cfRule type="endsWith" dxfId="6" priority="9" operator="endsWith" text="*">
-      <formula>RIGHT((D14),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E14:E16">
+    <cfRule type="endsWith" dxfId="7" priority="12" operator="endsWith" text="*">
+      <formula>RIGHT((E14),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D20">
-    <cfRule type="endsWith" dxfId="5" priority="8" operator="endsWith" text="*">
-      <formula>RIGHT((D18),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="endsWith" dxfId="6" priority="11" operator="endsWith" text="*">
+      <formula>RIGHT((E18),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D24">
-    <cfRule type="endsWith" dxfId="4" priority="7" operator="endsWith" text="*">
-      <formula>RIGHT((D22),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E22:E24">
+    <cfRule type="endsWith" dxfId="5" priority="10" operator="endsWith" text="*">
+      <formula>RIGHT((E22),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D28">
-    <cfRule type="endsWith" dxfId="3" priority="5" operator="endsWith" text="*">
-      <formula>RIGHT((D26),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E26:E28">
+    <cfRule type="endsWith" dxfId="4" priority="8" operator="endsWith" text="*">
+      <formula>RIGHT((E26),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D32">
-    <cfRule type="endsWith" dxfId="2" priority="6" operator="endsWith" text="*">
-      <formula>RIGHT((D30),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E30:E32">
+    <cfRule type="endsWith" dxfId="3" priority="9" operator="endsWith" text="*">
+      <formula>RIGHT((E30),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D37">
-    <cfRule type="endsWith" dxfId="1" priority="3" operator="endsWith" text="*">
-      <formula>RIGHT((D34),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E34:E37">
+    <cfRule type="endsWith" dxfId="2" priority="6" operator="endsWith" text="*">
+      <formula>RIGHT((E34),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D40">
-    <cfRule type="endsWith" dxfId="0" priority="1" operator="endsWith" text="*">
-      <formula>RIGHT((D39),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E39:E40">
+    <cfRule type="endsWith" dxfId="1" priority="4" operator="endsWith" text="*">
+      <formula>RIGHT((E39),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:C26">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD966"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C24">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD966"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C23">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(I22))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update vital skills and data mining
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3637FF8F-90B1-D94C-83CA-21901FA91644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F676CB7-4144-8947-BBCF-44EB3DA278D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="500" windowWidth="24820" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="500" windowWidth="16780" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="179">
   <si>
     <t>Course Code</t>
   </si>
@@ -571,17 +571,36 @@
   </si>
   <si>
     <t>15 courses where final is 20 percent or less</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>pct. Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">course </t>
+  </si>
+  <si>
+    <t>course desc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1059,435 +1078,435 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="14" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1496,50 +1515,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="21" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="32" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="13" fillId="21" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="13" fillId="32" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1548,55 +1567,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="81">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="75">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3290,42 +3261,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="endsWith" dxfId="80" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="74" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((D2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E22">
-    <cfRule type="containsText" dxfId="79" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="73" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="containsText" dxfId="78" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="72" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="71" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="beginsWith" dxfId="76" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="70" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((F2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="75" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="69" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((F2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G22">
-    <cfRule type="containsText" dxfId="74" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="66" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(F2))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3354,43 +3325,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J22">
-    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="64" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(J2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K11">
-    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:K16">
-    <cfRule type="containsText" dxfId="66" priority="166" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="166" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:K16 H15:H16 L12:L16 M15:M16">
-    <cfRule type="containsText" dxfId="65" priority="167" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="59" priority="167" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:K22">
-    <cfRule type="containsText" dxfId="64" priority="162" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="162" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L11 F15:G16">
-    <cfRule type="containsText" dxfId="63" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L22">
-    <cfRule type="containsText" dxfId="62" priority="164" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="56" priority="164" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(R12))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3966,47 +3937,47 @@
     <row r="36" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="endsWith" dxfId="61" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="55" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((C2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D17">
-    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="54" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="containsText" dxfId="59" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="53" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="beginsWith" dxfId="57" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="51" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((E2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="56" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="50" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((E2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F17">
-    <cfRule type="containsText" dxfId="55" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="49" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="48" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F5 K1 E16:F17">
-    <cfRule type="containsText" dxfId="51" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="45" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4035,98 +4006,98 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="44" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="42" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1 E5:F5">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J3">
-    <cfRule type="containsText" dxfId="46" priority="72" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="72" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4 G4 L4 K4:K7">
-    <cfRule type="containsText" dxfId="45" priority="36" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J7">
-    <cfRule type="containsText" dxfId="44" priority="35" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="38" priority="35" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:J7">
-    <cfRule type="containsText" dxfId="43" priority="199" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="199" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J10">
-    <cfRule type="containsText" dxfId="42" priority="128" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="128" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:J13">
-    <cfRule type="containsText" dxfId="41" priority="212" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="212" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J14">
-    <cfRule type="containsText" dxfId="40" priority="205" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="34" priority="205" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J15">
-    <cfRule type="containsText" dxfId="39" priority="124" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="124" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:J17">
-    <cfRule type="containsText" dxfId="38" priority="68" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="32" priority="68" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="37" priority="201" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="31" priority="201" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K10">
-    <cfRule type="containsText" dxfId="36" priority="130" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="30" priority="130" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K13">
-    <cfRule type="containsText" dxfId="35" priority="214" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="29" priority="214" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="34" priority="207" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="28" priority="207" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="33" priority="126" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="27" priority="126" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K17">
-    <cfRule type="containsText" dxfId="32" priority="70" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="26" priority="70" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2 K2:K3">
-    <cfRule type="containsText" dxfId="31" priority="73" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="25" priority="73" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q25))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4163,17 +4134,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="188"/>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
-      <c r="E1" s="189"/>
-      <c r="F1" s="189"/>
-      <c r="G1" s="189"/>
-      <c r="H1" s="189"/>
-      <c r="I1" s="189"/>
-      <c r="J1" s="189"/>
-      <c r="K1" s="189"/>
+      <c r="A1" s="197"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="198"/>
     </row>
     <row r="2" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -5380,15 +5351,15 @@
         <v>88</v>
       </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="190" t="s">
+      <c r="E35" s="199" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="189"/>
-      <c r="G35" s="189"/>
-      <c r="H35" s="189"/>
-      <c r="I35" s="189"/>
-      <c r="J35" s="189"/>
-      <c r="K35" s="189"/>
+      <c r="F35" s="198"/>
+      <c r="G35" s="198"/>
+      <c r="H35" s="198"/>
+      <c r="I35" s="198"/>
+      <c r="J35" s="198"/>
+      <c r="K35" s="198"/>
     </row>
     <row r="36" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38" t="s">
@@ -5401,15 +5372,15 @@
         <v>88</v>
       </c>
       <c r="D36" s="53"/>
-      <c r="E36" s="190" t="s">
+      <c r="E36" s="199" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="189"/>
-      <c r="G36" s="189"/>
-      <c r="H36" s="189"/>
-      <c r="I36" s="189"/>
-      <c r="J36" s="189"/>
-      <c r="K36" s="189"/>
+      <c r="F36" s="198"/>
+      <c r="G36" s="198"/>
+      <c r="H36" s="198"/>
+      <c r="I36" s="198"/>
+      <c r="J36" s="198"/>
+      <c r="K36" s="198"/>
     </row>
     <row r="37" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
@@ -5455,15 +5426,15 @@
         <v>88</v>
       </c>
       <c r="D38" s="52"/>
-      <c r="E38" s="190" t="s">
+      <c r="E38" s="199" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="189"/>
-      <c r="G38" s="189"/>
-      <c r="H38" s="189"/>
-      <c r="I38" s="189"/>
-      <c r="J38" s="189"/>
-      <c r="K38" s="189"/>
+      <c r="F38" s="198"/>
+      <c r="G38" s="198"/>
+      <c r="H38" s="198"/>
+      <c r="I38" s="198"/>
+      <c r="J38" s="198"/>
+      <c r="K38" s="198"/>
     </row>
     <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -5476,15 +5447,15 @@
         <v>88</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="191" t="s">
+      <c r="E39" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="192"/>
-      <c r="G39" s="192"/>
-      <c r="H39" s="192"/>
-      <c r="I39" s="192"/>
-      <c r="J39" s="192"/>
-      <c r="K39" s="192"/>
+      <c r="F39" s="201"/>
+      <c r="G39" s="201"/>
+      <c r="H39" s="201"/>
+      <c r="I39" s="201"/>
+      <c r="J39" s="201"/>
+      <c r="K39" s="201"/>
     </row>
     <row r="40" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="63" t="s">
@@ -14338,7 +14309,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{75BAD67C-9351-3043-9100-0313E659D61F}">
+      <autoFilter ref="A2:K42" xr:uid="{4866CFC3-0FE3-2446-97EC-BEFE97443051}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -14355,42 +14326,42 @@
     <mergeCell ref="E39:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="endsWith" dxfId="30" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="24" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C42">
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D42">
-    <cfRule type="beginsWith" dxfId="26" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="20" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((D3),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="19" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D3),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E42 G36">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14419,25 +14390,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H37 H40:H42">
-    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H40:H42 H37">
-    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I34 D26:E26 D35 H37:I37 H40:I1012 D41:E41">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I23 D26:F26 H26:I26 D35 H40:I40 D40:E41 J1:J34 D22:F23 K22:K24 K26 D32:E33 J37 F40 K40 J40:J1012">
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14451,8 +14422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF7805C-9A25-014E-8DE3-513BC4007718}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14466,7 +14437,7 @@
     <col min="7" max="7" width="13.33203125" style="185" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="185"/>
     <col min="10" max="10" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5" style="185" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="185" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.83203125" style="185" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="185"/>
@@ -14494,68 +14465,93 @@
       <c r="H1" s="185" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="202"/>
+      <c r="J1" s="185" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" s="185" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="187" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" s="185" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="185">
+        <v>1</v>
+      </c>
+      <c r="K2" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="185" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="190" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="185" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="193" t="s">
+      <c r="B3" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="197">
+      <c r="C3" s="192">
         <v>0.16</v>
       </c>
-      <c r="D3" s="193" t="s">
+      <c r="D3" s="188" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="194" t="s">
+      <c r="E3" s="189" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="185" t="s">
         <v>158</v>
       </c>
       <c r="J3" s="185">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K3" s="187">
         <v>0.5</v>
       </c>
       <c r="L3" s="185" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="195" t="s">
-        <v>39</v>
+        <v>83</v>
+      </c>
+      <c r="M3" s="190" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J4" s="185">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K4" s="187">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="L4" s="185" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="195" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+      <c r="M4" s="190" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="185" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="197">
+      <c r="C5" s="192">
         <v>0.17</v>
       </c>
-      <c r="D5" s="193" t="s">
+      <c r="D5" s="188" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="194" t="s">
+      <c r="E5" s="189" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="185" t="s">
@@ -14565,29 +14561,29 @@
         <v>34</v>
       </c>
       <c r="J5" s="185">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="187">
-        <v>0.28000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="L5" s="185" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="195" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="M5" s="190" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="193" t="s">
+      <c r="B6" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="197">
+      <c r="C6" s="192">
         <v>0.1</v>
       </c>
-      <c r="D6" s="193" t="s">
+      <c r="D6" s="188" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="194" t="s">
+      <c r="E6" s="189" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="185" t="s">
@@ -14597,30 +14593,30 @@
         <v>38</v>
       </c>
       <c r="J6" s="185">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K6" s="187">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="L6" s="185" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="195" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="M6" s="190" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J7" s="185">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K7" s="187">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="L7" s="185" t="s">
-        <v>83</v>
-      </c>
-      <c r="M7" s="195" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="M7" s="190" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14636,7 +14632,7 @@
       <c r="D8" s="185" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="195" t="s">
+      <c r="E8" s="190" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="185" t="s">
@@ -14646,16 +14642,16 @@
         <v>158</v>
       </c>
       <c r="J8" s="185">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K8" s="187">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="L8" s="185" t="s">
-        <v>86</v>
-      </c>
-      <c r="M8" s="195" t="s">
-        <v>87</v>
+        <v>118</v>
+      </c>
+      <c r="M8" s="191" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14668,37 +14664,37 @@
       <c r="D9" s="185" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="195" t="s">
+      <c r="E9" s="190" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="185" t="s">
         <v>158</v>
       </c>
       <c r="J9" s="185">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K9" s="187">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="L9" s="185" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="195" t="s">
-        <v>25</v>
+        <v>77</v>
+      </c>
+      <c r="M9" s="190" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J10" s="185">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K10" s="187">
-        <v>0.22</v>
+        <v>0.3</v>
       </c>
       <c r="L10" s="185" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="195" t="s">
-        <v>36</v>
+        <v>89</v>
+      </c>
+      <c r="M10" s="190" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14714,7 +14710,7 @@
       <c r="D11" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="195" t="s">
+      <c r="E11" s="190" t="s">
         <v>45</v>
       </c>
       <c r="F11" s="185" t="s">
@@ -14724,16 +14720,16 @@
         <v>158</v>
       </c>
       <c r="J11" s="185">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K11" s="187">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="L11" s="185" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="195" t="s">
-        <v>75</v>
+        <v>86</v>
+      </c>
+      <c r="M11" s="190" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14746,37 +14742,37 @@
       <c r="D12" s="185" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="195" t="s">
+      <c r="E12" s="190" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="185" t="s">
         <v>158</v>
       </c>
       <c r="J12" s="185">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K12" s="187">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L12" s="185" t="s">
-        <v>77</v>
-      </c>
-      <c r="M12" s="195" t="s">
-        <v>78</v>
+        <v>44</v>
+      </c>
+      <c r="M12" s="190" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J13" s="185">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K13" s="187">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="L13" s="185" t="s">
-        <v>79</v>
-      </c>
-      <c r="M13" s="195" t="s">
-        <v>80</v>
+        <v>24</v>
+      </c>
+      <c r="M13" s="190" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14786,13 +14782,13 @@
       <c r="B14" s="185" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="198">
+      <c r="C14" s="193">
         <v>0.2</v>
       </c>
-      <c r="D14" s="199" t="s">
+      <c r="D14" s="194" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="201" t="s">
+      <c r="E14" s="196" t="s">
         <v>82</v>
       </c>
       <c r="F14" s="185" t="s">
@@ -14802,16 +14798,16 @@
         <v>158</v>
       </c>
       <c r="J14" s="185">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K14" s="187">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="L14" s="185" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="195" t="s">
-        <v>90</v>
+        <v>35</v>
+      </c>
+      <c r="M14" s="190" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14824,7 +14820,7 @@
       <c r="D15" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="195" t="s">
+      <c r="E15" s="190" t="s">
         <v>84</v>
       </c>
       <c r="F15" s="185" t="s">
@@ -14832,18 +14828,6 @@
       </c>
       <c r="G15" s="185" t="s">
         <v>158</v>
-      </c>
-      <c r="J15" s="185">
-        <v>13</v>
-      </c>
-      <c r="K15" s="187">
-        <v>0.31</v>
-      </c>
-      <c r="L15" s="185" t="s">
-        <v>118</v>
-      </c>
-      <c r="M15" s="196" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14856,11 +14840,16 @@
       <c r="D16" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="195" t="s">
+      <c r="E16" s="190" t="s">
         <v>87</v>
       </c>
       <c r="G16" s="185" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="185" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -14876,7 +14865,7 @@
       <c r="D18" s="185" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="195" t="s">
+      <c r="E18" s="190" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="185" t="s">
@@ -14884,22 +14873,19 @@
       </c>
       <c r="G18" s="185" t="s">
         <v>158</v>
-      </c>
-      <c r="J18" s="185" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="198">
+      <c r="C19" s="193">
         <v>0.2</v>
       </c>
-      <c r="D19" s="199" t="s">
+      <c r="D19" s="194" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="201" t="s">
+      <c r="E19" s="196" t="s">
         <v>32</v>
       </c>
       <c r="G19" s="185" t="s">
@@ -14916,7 +14902,7 @@
       <c r="D20" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="195" t="s">
+      <c r="E20" s="190" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="185" t="s">
@@ -14941,7 +14927,7 @@
       <c r="D22" s="185" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="195" t="s">
+      <c r="E22" s="190" t="s">
         <v>75</v>
       </c>
       <c r="G22" s="185" t="s">
@@ -14958,7 +14944,7 @@
       <c r="D23" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="195" t="s">
+      <c r="E23" s="190" t="s">
         <v>78</v>
       </c>
       <c r="G23" s="185" t="s">
@@ -14975,7 +14961,7 @@
       <c r="D24" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="195" t="s">
+      <c r="E24" s="190" t="s">
         <v>80</v>
       </c>
       <c r="G24" s="185" t="s">
@@ -14989,13 +14975,13 @@
       <c r="B26" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="198">
+      <c r="C26" s="193">
         <v>0.2</v>
       </c>
-      <c r="D26" s="200" t="s">
+      <c r="D26" s="195" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="201" t="s">
+      <c r="E26" s="196" t="s">
         <v>66</v>
       </c>
       <c r="G26" s="185" t="s">
@@ -15006,13 +14992,13 @@
       <c r="B27" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="198">
+      <c r="C27" s="193">
         <v>0.2</v>
       </c>
-      <c r="D27" s="200" t="s">
+      <c r="D27" s="195" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="201" t="s">
+      <c r="E27" s="196" t="s">
         <v>70</v>
       </c>
       <c r="G27" s="185" t="s">
@@ -15023,13 +15009,13 @@
       <c r="B28" s="185" t="s">
         <v>167</v>
       </c>
-      <c r="C28" s="198">
+      <c r="C28" s="193">
         <v>0.1</v>
       </c>
-      <c r="D28" s="200" t="s">
+      <c r="D28" s="195" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="201" t="s">
+      <c r="E28" s="196" t="s">
         <v>72</v>
       </c>
       <c r="G28" s="185" t="s">
@@ -15043,13 +15029,13 @@
       <c r="B30" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="198">
+      <c r="C30" s="193">
         <v>0.2</v>
       </c>
-      <c r="D30" s="199" t="s">
+      <c r="D30" s="194" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="201" t="s">
+      <c r="E30" s="202" t="s">
         <v>56</v>
       </c>
       <c r="G30" s="185" t="s">
@@ -15060,13 +15046,13 @@
       <c r="B31" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="198">
+      <c r="C31" s="193">
         <v>0.2</v>
       </c>
-      <c r="D31" s="199" t="s">
+      <c r="D31" s="194" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="201" t="s">
+      <c r="E31" s="196" t="s">
         <v>60</v>
       </c>
       <c r="G31" s="185" t="s">
@@ -15077,13 +15063,13 @@
       <c r="B32" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="198">
+      <c r="C32" s="193">
         <v>0.2</v>
       </c>
-      <c r="D32" s="199" t="s">
+      <c r="D32" s="194" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="201" t="s">
+      <c r="E32" s="196" t="s">
         <v>63</v>
       </c>
       <c r="G32" s="185" t="s">
@@ -15103,7 +15089,7 @@
       <c r="D34" s="185" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="195" t="s">
+      <c r="E34" s="190" t="s">
         <v>90</v>
       </c>
       <c r="G34" s="185" t="s">
@@ -15114,13 +15100,13 @@
       <c r="B35" s="185" t="s">
         <v>168</v>
       </c>
-      <c r="C35" s="198">
+      <c r="C35" s="193">
         <v>0.2</v>
       </c>
-      <c r="D35" s="199" t="s">
+      <c r="D35" s="194" t="s">
         <v>124</v>
       </c>
-      <c r="E35" s="200" t="s">
+      <c r="E35" s="195" t="s">
         <v>125</v>
       </c>
       <c r="G35" s="185" t="s">
@@ -15131,13 +15117,13 @@
       <c r="B36" s="185" t="s">
         <v>168</v>
       </c>
-      <c r="C36" s="198">
+      <c r="C36" s="193">
         <v>0.2</v>
       </c>
-      <c r="D36" s="199" t="s">
+      <c r="D36" s="194" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="200" t="s">
+      <c r="E36" s="195" t="s">
         <v>127</v>
       </c>
       <c r="G36" s="185" t="s">
@@ -15148,13 +15134,13 @@
       <c r="B37" s="185" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="198">
+      <c r="C37" s="193">
         <v>0.2</v>
       </c>
-      <c r="D37" s="199" t="s">
+      <c r="D37" s="194" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="200" t="s">
+      <c r="E37" s="195" t="s">
         <v>129</v>
       </c>
       <c r="G37" s="185" t="s">
@@ -15174,7 +15160,7 @@
       <c r="D39" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="196" t="s">
+      <c r="E39" s="191" t="s">
         <v>119</v>
       </c>
       <c r="G39" s="185" t="s">
@@ -15185,13 +15171,13 @@
       <c r="B40" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="198">
+      <c r="C40" s="193">
         <v>0.1</v>
       </c>
-      <c r="D40" s="199" t="s">
+      <c r="D40" s="194" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="200" t="s">
+      <c r="E40" s="195" t="s">
         <v>112</v>
       </c>
       <c r="G40" s="185" t="s">
@@ -15199,84 +15185,54 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3 E5:E6 M9:M10">
-    <cfRule type="endsWith" dxfId="15" priority="21" operator="endsWith" text="*">
-      <formula>RIGHT((E3),LEN("*"))=("*")</formula>
+  <conditionalFormatting sqref="E3 E5:E6 M2:M14">
+    <cfRule type="endsWith" dxfId="9" priority="21" operator="endsWith" text="*">
+      <formula>RIGHT((E2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E9">
-    <cfRule type="endsWith" dxfId="14" priority="20" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="8" priority="20" operator="endsWith" text="*">
       <formula>RIGHT((E8),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E12">
-    <cfRule type="endsWith" dxfId="13" priority="19" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="7" priority="19" operator="endsWith" text="*">
       <formula>RIGHT((E11),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E16">
-    <cfRule type="endsWith" dxfId="12" priority="18" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="6" priority="18" operator="endsWith" text="*">
       <formula>RIGHT((E14),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E20">
-    <cfRule type="endsWith" dxfId="11" priority="17" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="5" priority="17" operator="endsWith" text="*">
       <formula>RIGHT((E18),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E24">
-    <cfRule type="endsWith" dxfId="10" priority="16" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="4" priority="16" operator="endsWith" text="*">
       <formula>RIGHT((E22),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E28">
-    <cfRule type="endsWith" dxfId="9" priority="14" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="3" priority="14" operator="endsWith" text="*">
       <formula>RIGHT((E26),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E32">
-    <cfRule type="endsWith" dxfId="8" priority="15" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="2" priority="15" operator="endsWith" text="*">
       <formula>RIGHT((E30),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E37">
-    <cfRule type="endsWith" dxfId="7" priority="13" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="1" priority="13" operator="endsWith" text="*">
       <formula>RIGHT((E34),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E40">
-    <cfRule type="endsWith" dxfId="6" priority="12" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="0" priority="12" operator="endsWith" text="*">
       <formula>RIGHT((E39),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M4">
-    <cfRule type="endsWith" dxfId="5" priority="7" operator="endsWith" text="*">
-      <formula>RIGHT((M3),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M6">
-    <cfRule type="endsWith" dxfId="4" priority="6" operator="endsWith" text="*">
-      <formula>RIGHT((M5),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M7:M8">
-    <cfRule type="endsWith" dxfId="3" priority="5" operator="endsWith" text="*">
-      <formula>RIGHT((M7),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M13">
-    <cfRule type="endsWith" dxfId="2" priority="3" operator="endsWith" text="*">
-      <formula>RIGHT((M11),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14">
-    <cfRule type="endsWith" dxfId="1" priority="2" operator="endsWith" text="*">
-      <formula>RIGHT((M14),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M15">
-    <cfRule type="endsWith" dxfId="0" priority="1" operator="endsWith" text="*">
-      <formula>RIGHT((M15),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update data mining proj
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F676CB7-4144-8947-BBCF-44EB3DA278D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494CE952-D24B-5F47-88DF-A4A3D65E315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="500" windowWidth="16780" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14460" yWindow="500" windowWidth="19140" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
     <sheet name="Electives" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
     <sheet name="Schedule" sheetId="5" r:id="rId4"/>
+    <sheet name="Schedule 2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$2:$K$42</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="179">
   <si>
     <t>Course Code</t>
   </si>
@@ -589,7 +590,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -693,8 +694,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,6 +893,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,7 +1096,7 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1547,6 +1562,9 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1558,16 +1576,80 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="14" fillId="33" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="82">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3261,42 +3343,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="endsWith" dxfId="74" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="81" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((D2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E22">
-    <cfRule type="containsText" dxfId="73" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="80" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="containsText" dxfId="72" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="79" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="78" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="beginsWith" dxfId="70" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="77" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((F2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="69" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="76" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((F2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G22">
-    <cfRule type="containsText" dxfId="68" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="74" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(F2))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3325,43 +3407,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J22">
-    <cfRule type="containsText" dxfId="64" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="71" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="70" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="69" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(J2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K11">
-    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:K16">
-    <cfRule type="containsText" dxfId="60" priority="166" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="67" priority="166" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:K16 H15:H16 L12:L16 M15:M16">
-    <cfRule type="containsText" dxfId="59" priority="167" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="66" priority="167" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:K22">
-    <cfRule type="containsText" dxfId="58" priority="162" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="65" priority="162" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L11 F15:G16">
-    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L22">
-    <cfRule type="containsText" dxfId="56" priority="164" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="63" priority="164" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(R12))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3937,47 +4019,47 @@
     <row r="36" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="endsWith" dxfId="55" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="62" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((C2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D17">
-    <cfRule type="containsText" dxfId="54" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="61" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="containsText" dxfId="53" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="60" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="59" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="beginsWith" dxfId="51" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="58" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((E2),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="50" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="57" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((E2),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F17">
-    <cfRule type="containsText" dxfId="49" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="56" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="54" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="53" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F5 K1 E16:F17">
-    <cfRule type="containsText" dxfId="45" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4006,98 +4088,98 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="containsText" dxfId="44" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="51" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="50" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="49" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1 E5:F5">
-    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="48" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J3">
-    <cfRule type="containsText" dxfId="40" priority="72" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="47" priority="72" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4 G4 L4 K4:K7">
-    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="46" priority="36" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J7">
-    <cfRule type="containsText" dxfId="38" priority="35" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="45" priority="35" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:J7">
-    <cfRule type="containsText" dxfId="37" priority="199" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="44" priority="199" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J10">
-    <cfRule type="containsText" dxfId="36" priority="128" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="128" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:J13">
-    <cfRule type="containsText" dxfId="35" priority="212" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="42" priority="212" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J14">
-    <cfRule type="containsText" dxfId="34" priority="205" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="41" priority="205" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J15">
-    <cfRule type="containsText" dxfId="33" priority="124" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="40" priority="124" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:J17">
-    <cfRule type="containsText" dxfId="32" priority="68" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="39" priority="68" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="31" priority="201" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="38" priority="201" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K10">
-    <cfRule type="containsText" dxfId="30" priority="130" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="37" priority="130" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K13">
-    <cfRule type="containsText" dxfId="29" priority="214" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="36" priority="214" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="28" priority="207" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="35" priority="207" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="27" priority="126" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="34" priority="126" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K17">
-    <cfRule type="containsText" dxfId="26" priority="70" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="33" priority="70" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2 K2:K3">
-    <cfRule type="containsText" dxfId="25" priority="73" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="32" priority="73" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q25))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4134,17 +4216,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="197"/>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
+      <c r="A1" s="198"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
     </row>
     <row r="2" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -5351,15 +5433,15 @@
         <v>88</v>
       </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="199" t="s">
+      <c r="E35" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="198"/>
-      <c r="G35" s="198"/>
-      <c r="H35" s="198"/>
-      <c r="I35" s="198"/>
-      <c r="J35" s="198"/>
-      <c r="K35" s="198"/>
+      <c r="F35" s="199"/>
+      <c r="G35" s="199"/>
+      <c r="H35" s="199"/>
+      <c r="I35" s="199"/>
+      <c r="J35" s="199"/>
+      <c r="K35" s="199"/>
     </row>
     <row r="36" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38" t="s">
@@ -5372,15 +5454,15 @@
         <v>88</v>
       </c>
       <c r="D36" s="53"/>
-      <c r="E36" s="199" t="s">
+      <c r="E36" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="198"/>
-      <c r="G36" s="198"/>
-      <c r="H36" s="198"/>
-      <c r="I36" s="198"/>
-      <c r="J36" s="198"/>
-      <c r="K36" s="198"/>
+      <c r="F36" s="199"/>
+      <c r="G36" s="199"/>
+      <c r="H36" s="199"/>
+      <c r="I36" s="199"/>
+      <c r="J36" s="199"/>
+      <c r="K36" s="199"/>
     </row>
     <row r="37" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
@@ -5426,15 +5508,15 @@
         <v>88</v>
       </c>
       <c r="D38" s="52"/>
-      <c r="E38" s="199" t="s">
+      <c r="E38" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="198"/>
-      <c r="G38" s="198"/>
-      <c r="H38" s="198"/>
-      <c r="I38" s="198"/>
-      <c r="J38" s="198"/>
-      <c r="K38" s="198"/>
+      <c r="F38" s="199"/>
+      <c r="G38" s="199"/>
+      <c r="H38" s="199"/>
+      <c r="I38" s="199"/>
+      <c r="J38" s="199"/>
+      <c r="K38" s="199"/>
     </row>
     <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -5447,15 +5529,15 @@
         <v>88</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="200" t="s">
+      <c r="E39" s="201" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="201"/>
-      <c r="G39" s="201"/>
-      <c r="H39" s="201"/>
-      <c r="I39" s="201"/>
-      <c r="J39" s="201"/>
-      <c r="K39" s="201"/>
+      <c r="F39" s="202"/>
+      <c r="G39" s="202"/>
+      <c r="H39" s="202"/>
+      <c r="I39" s="202"/>
+      <c r="J39" s="202"/>
+      <c r="K39" s="202"/>
     </row>
     <row r="40" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="63" t="s">
@@ -14309,7 +14391,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{4866CFC3-0FE3-2446-97EC-BEFE97443051}">
+      <autoFilter ref="A2:K42" xr:uid="{343C4DD0-6B70-7D46-921F-327F6C0AFD21}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -14326,42 +14408,42 @@
     <mergeCell ref="E39:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="endsWith" dxfId="24" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="31" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C42">
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D42">
-    <cfRule type="beginsWith" dxfId="20" priority="16" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="27" priority="16" operator="beginsWith" text="R">
       <formula>LEFT((D3),LEN("R"))=("R")</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="26" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D3),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E42 G36">
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14390,25 +14472,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H37 H40:H42">
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="20" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H40:H42 H37">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I34 D26:E26 D35 H37:I37 H40:I1012 D41:E41">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I23 D26:F26 H26:I26 D35 H40:I40 D40:E41 J1:J34 D22:F23 K22:K24 K26 D32:E33 J37 F40 K40 J40:J1012">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14422,8 +14504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF7805C-9A25-014E-8DE3-513BC4007718}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D46" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15035,7 +15117,7 @@
       <c r="D30" s="194" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="202" t="s">
+      <c r="E30" s="197" t="s">
         <v>56</v>
       </c>
       <c r="G30" s="185" t="s">
@@ -15185,54 +15267,858 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3 E5:E6 M2:M14">
-    <cfRule type="endsWith" dxfId="9" priority="21" operator="endsWith" text="*">
-      <formula>RIGHT((E2),LEN("*"))=("*")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E8:E9">
-    <cfRule type="endsWith" dxfId="8" priority="20" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="16" priority="20" operator="endsWith" text="*">
       <formula>RIGHT((E8),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E12">
-    <cfRule type="endsWith" dxfId="7" priority="19" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="15" priority="19" operator="endsWith" text="*">
       <formula>RIGHT((E11),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E16">
-    <cfRule type="endsWith" dxfId="6" priority="18" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="14" priority="18" operator="endsWith" text="*">
       <formula>RIGHT((E14),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E20">
-    <cfRule type="endsWith" dxfId="5" priority="17" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="13" priority="17" operator="endsWith" text="*">
       <formula>RIGHT((E18),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E24">
-    <cfRule type="endsWith" dxfId="4" priority="16" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="12" priority="16" operator="endsWith" text="*">
       <formula>RIGHT((E22),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E28">
-    <cfRule type="endsWith" dxfId="3" priority="14" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="11" priority="14" operator="endsWith" text="*">
       <formula>RIGHT((E26),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E32">
-    <cfRule type="endsWith" dxfId="2" priority="15" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="10" priority="15" operator="endsWith" text="*">
       <formula>RIGHT((E30),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E37">
-    <cfRule type="endsWith" dxfId="1" priority="13" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="9" priority="13" operator="endsWith" text="*">
       <formula>RIGHT((E34),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:E40">
-    <cfRule type="endsWith" dxfId="0" priority="12" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="8" priority="12" operator="endsWith" text="*">
       <formula>RIGHT((E39),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M14 E3 E5:E6">
+    <cfRule type="endsWith" dxfId="7" priority="21" operator="endsWith" text="*">
+      <formula>RIGHT((E2),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A2002B0-CD3E-3243-9D7D-6B4B46807CF5}">
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="185" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="185"/>
+    <col min="3" max="3" width="11.6640625" style="187" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.1640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="185" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="185"/>
+    <col min="10" max="10" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.83203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="185"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="206" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="206" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="206" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="207" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="206" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="206" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="206" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="206" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="206" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" s="206" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="207" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" s="206" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="185">
+        <v>1</v>
+      </c>
+      <c r="K2" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="185" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="190" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="185" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="188" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="192">
+        <v>0.16</v>
+      </c>
+      <c r="D3" s="188" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="189" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J3" s="185">
+        <v>5</v>
+      </c>
+      <c r="K3" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="185" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="190" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="185">
+        <v>11</v>
+      </c>
+      <c r="K4" s="187">
+        <v>0.45</v>
+      </c>
+      <c r="L4" s="185" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="190" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="185" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="188" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="192">
+        <v>0.17</v>
+      </c>
+      <c r="D5" s="188" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="189" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="185">
+        <v>34</v>
+      </c>
+      <c r="J5" s="185">
+        <v>4</v>
+      </c>
+      <c r="K5" s="187">
+        <v>0.4</v>
+      </c>
+      <c r="L5" s="185" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="190" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="188" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="192">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="188" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="189" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="185">
+        <v>38</v>
+      </c>
+      <c r="J6" s="185">
+        <v>2</v>
+      </c>
+      <c r="K6" s="187">
+        <v>0.35</v>
+      </c>
+      <c r="L6" s="185" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="190" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="185">
+        <v>9</v>
+      </c>
+      <c r="K7" s="187">
+        <v>0.33</v>
+      </c>
+      <c r="L7" s="185" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="190" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="185" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="185" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="190" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="185" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="185">
+        <v>13</v>
+      </c>
+      <c r="K8" s="187">
+        <v>0.31</v>
+      </c>
+      <c r="L8" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="M8" s="191" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="187">
+        <v>0.35</v>
+      </c>
+      <c r="D9" s="185" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="190" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J9" s="185">
+        <v>10</v>
+      </c>
+      <c r="K9" s="187">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="185" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="190" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="187">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D10" s="185" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="190" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J10" s="185">
+        <v>12</v>
+      </c>
+      <c r="K10" s="187">
+        <v>0.3</v>
+      </c>
+      <c r="L10" s="185" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="190" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="190"/>
+      <c r="K11" s="187"/>
+      <c r="M11" s="190"/>
+    </row>
+    <row r="12" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="185" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="187">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="185" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="190" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="185">
+        <v>6</v>
+      </c>
+      <c r="K12" s="187">
+        <v>0.3</v>
+      </c>
+      <c r="L12" s="185" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="190" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="187">
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="185" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="190" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J13" s="185">
+        <v>3</v>
+      </c>
+      <c r="K13" s="187">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L13" s="185" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="190" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="194" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="196" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J14" s="185">
+        <v>7</v>
+      </c>
+      <c r="K14" s="187">
+        <v>0.25</v>
+      </c>
+      <c r="L14" s="185" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="190" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="203" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="204"/>
+      <c r="E15" s="205"/>
+      <c r="K15" s="204"/>
+      <c r="M15" s="205"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="185" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="194" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="196" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="185" t="s">
+        <v>158</v>
+      </c>
+      <c r="J16" s="185">
+        <v>8</v>
+      </c>
+      <c r="K16" s="187">
+        <v>0.22</v>
+      </c>
+      <c r="L16" s="185" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="190" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="187">
+        <v>0.22</v>
+      </c>
+      <c r="D17" s="185" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="190" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="185"/>
+    </row>
+    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="185" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="185" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="190" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="187">
+        <v>0.3</v>
+      </c>
+      <c r="D20" s="185" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="190" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="185"/>
+    </row>
+    <row r="22" spans="1:7" s="209" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="208" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="210"/>
+    </row>
+    <row r="23" spans="1:7" s="203" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="211"/>
+      <c r="C23" s="204"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="185" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="187">
+        <v>0.33</v>
+      </c>
+      <c r="D24" s="185" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="190" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="187">
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="185" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="190" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="187">
+        <v>0.45</v>
+      </c>
+      <c r="D26" s="185" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="190" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="185" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D28" s="195" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="196" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="195" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="196" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="193">
+        <v>0.1</v>
+      </c>
+      <c r="D30" s="195" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="196" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="185" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="194" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="197" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="194" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="196" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D34" s="194" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="196" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="185" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="185" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="185" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="187">
+        <v>0.3</v>
+      </c>
+      <c r="D36" s="185" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="190" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D37" s="194" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="195" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D38" s="194" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="195" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="193">
+        <v>0.2</v>
+      </c>
+      <c r="D39" s="194" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="195" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="185" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="185" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="187">
+        <v>0.31</v>
+      </c>
+      <c r="D41" s="185" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="191" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="193">
+        <v>0.1</v>
+      </c>
+      <c r="D42" s="194" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="195" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="185" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E19:E20 E8:E17">
+    <cfRule type="endsWith" dxfId="6" priority="9" operator="endsWith" text="*">
+      <formula>RIGHT((E8),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E26">
+    <cfRule type="endsWith" dxfId="5" priority="5" operator="endsWith" text="*">
+      <formula>RIGHT((E24),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:E30">
+    <cfRule type="endsWith" dxfId="4" priority="3" operator="endsWith" text="*">
+      <formula>RIGHT((E28),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32:E34">
+    <cfRule type="endsWith" dxfId="3" priority="4" operator="endsWith" text="*">
+      <formula>RIGHT((E32),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36:E39">
+    <cfRule type="endsWith" dxfId="2" priority="2" operator="endsWith" text="*">
+      <formula>RIGHT((E36),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41:E42">
+    <cfRule type="endsWith" dxfId="1" priority="1" operator="endsWith" text="*">
+      <formula>RIGHT((E41),LEN("*"))=("*")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M16 E3 E5:E6">
+    <cfRule type="endsWith" dxfId="0" priority="10" operator="endsWith" text="*">
+      <formula>RIGHT((E2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update data science course
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C104D4E2-C20E-634B-9350-3ADB6C50566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950D1D93-F159-3A4B-AF95-600CA8D18BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="500" windowWidth="19140" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12560" yWindow="500" windowWidth="19140" windowHeight="20500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory Courses" sheetId="3" r:id="rId1"/>
@@ -2491,7 +2491,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="A9:XFD9"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14531,7 +14531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF7805C-9A25-014E-8DE3-513BC4007718}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -16156,8 +16156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270BECA4-6AAE-274B-B7D6-00511C3836D6}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update excel and gen ai
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E3D69A-706B-494F-8D2B-F3DBA7FB7EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2DDF46-E66E-5448-BD9D-9541DA3FA17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="500" windowWidth="19140" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12540" yWindow="500" windowWidth="21060" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="178">
   <si>
     <t>Course Code</t>
   </si>
@@ -510,18 +510,6 @@
   </si>
   <si>
     <t>start study for 5001 - 5003</t>
-  </si>
-  <si>
-    <t>take 5001 - if ready</t>
-  </si>
-  <si>
-    <t>take 5001 or 5002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drop  5735  </t>
-  </si>
-  <si>
-    <t>take 5735</t>
   </si>
   <si>
     <t>C</t>
@@ -1762,126 +1750,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFFD966"/>
           <bgColor rgb="FFFFD966"/>
         </patternFill>
@@ -2010,8 +1878,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2026,8 +1894,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2042,8 +1910,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFD5A6BD"/>
           <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2058,16 +1942,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2082,8 +1958,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFEAD1DC"/>
-          <bgColor rgb="FFEAD1DC"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2092,14 +1968,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFEA9999"/>
           <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2170,8 +2038,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2186,8 +2054,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2202,8 +2078,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2218,8 +2094,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2234,8 +2110,120 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFEAD1DC"/>
           <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12684,7 +12672,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{4F54D17E-3B6B-684A-904F-90DF787C4A40}">
+      <autoFilter ref="A2:K42" xr:uid="{A6A99558-41E4-4842-B288-E5D3D04B07DD}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -12701,42 +12689,42 @@
     <mergeCell ref="E39:K39"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B42">
-    <cfRule type="endsWith" dxfId="29" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="79" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((B3),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1012">
-    <cfRule type="containsText" dxfId="28" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="78" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C42">
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="77" priority="8" operator="containsText" text="pathway">
+      <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(C3))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="pathway">
-      <formula>NOT(ISERROR(SEARCH(("pathway"),(C3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D42">
-    <cfRule type="beginsWith" dxfId="25" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="75" priority="16" operator="beginsWith" text="R">
+      <formula>LEFT((D3),LEN("R"))=("R")</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="74" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((D3),LEN("Python"))=("Python")</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="16" operator="beginsWith" text="R">
-      <formula>LEFT((D3),LEN("R"))=("R")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E42 G36">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Project">
+      <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(D3))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="Project">
-      <formula>NOT(ISERROR(SEARCH(("Project"),(D3))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(D3))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(D3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12765,25 +12753,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H37 H40:H42">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="I">
+    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="B">
+      <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="13" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(H3))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="B">
-      <formula>NOT(ISERROR(SEARCH(("B"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H34 H40:H42 H37">
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(H3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I34 D26:E26 D35 H37:I37 H40:I1012 D41:E41">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I23 D26:F26 H26:I26 D35 H40:I40 D40:E41 J1:J34 D22:F23 K22:K24 K26 D32:E33 J37 F40 K40 J40:J1012">
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12816,7 +12804,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>134</v>
@@ -12942,7 +12930,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="142" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E4" s="108" t="s">
         <v>13</v>
@@ -13056,7 +13044,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="142" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E7" s="108" t="s">
         <v>26</v>
@@ -13634,7 +13622,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="173" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B23" s="173" t="s">
         <v>136</v>
@@ -13677,43 +13665,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D22">
-    <cfRule type="endsWith" dxfId="79" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="64" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((D2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E22">
-    <cfRule type="containsText" dxfId="78" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="63" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="containsText" dxfId="77" priority="8" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="62" priority="8" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="61" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="beginsWith" dxfId="75" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="60" priority="16" operator="beginsWith" text="R">
+      <formula>LEFT((F2),LEN("R"))=("R")</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="59" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((F2),LEN("Python"))=("Python")</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="74" priority="16" operator="beginsWith" text="R">
-      <formula>LEFT((F2),LEN("R"))=("R")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G22">
-    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="58" priority="3" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(F2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(F2))))</formula>
+    <cfRule type="containsText" dxfId="56" priority="5" operator="containsText" text="Exam">
+      <formula>NOT(ISERROR(SEARCH(("Exam"),(F2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="6" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="55" priority="6" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(F2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="Exam">
-      <formula>NOT(ISERROR(SEARCH(("Exam"),(F2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H22">
@@ -13741,47 +13729,48 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J22">
-    <cfRule type="containsText" dxfId="69" priority="13" operator="containsText" text="I">
-      <formula>NOT(ISERROR(SEARCH(("I"),(J2))))</formula>
+    <cfRule type="containsText" dxfId="54" priority="11" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="53" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(J2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(J2))))</formula>
+    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="I">
+      <formula>NOT(ISERROR(SEARCH(("I"),(J2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K11">
-    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:K16">
-    <cfRule type="containsText" dxfId="65" priority="166" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="50" priority="166" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:K16 H15:H16 L12:L16 M15:M16">
-    <cfRule type="containsText" dxfId="64" priority="167" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="49" priority="167" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(N18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:K22">
-    <cfRule type="containsText" dxfId="63" priority="162" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="48" priority="162" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(N12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L11 F15:G16">
-    <cfRule type="containsText" dxfId="62" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L22">
-    <cfRule type="containsText" dxfId="61" priority="164" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="46" priority="164" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(R12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -14325,7 +14314,7 @@
     </row>
     <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="172" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14353,47 +14342,47 @@
     <row r="36" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="endsWith" dxfId="60" priority="10" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="45" priority="10" operator="endsWith" text="*">
       <formula>RIGHT((C2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D17">
-    <cfRule type="containsText" dxfId="59" priority="15" operator="containsText" text="Elective">
+    <cfRule type="containsText" dxfId="44" priority="15" operator="containsText" text="Elective">
       <formula>NOT(ISERROR(SEARCH(("Elective"),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="containsText" dxfId="58" priority="9" operator="containsText" text="Core">
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="pathway">
+      <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="Core">
       <formula>NOT(ISERROR(SEARCH(("Core"),(D2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="8" operator="containsText" text="pathway">
-      <formula>NOT(ISERROR(SEARCH(("pathway"),(D2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="beginsWith" dxfId="56" priority="17" operator="beginsWith" text="Python">
+    <cfRule type="beginsWith" dxfId="41" priority="16" operator="beginsWith" text="R">
+      <formula>LEFT((E2),LEN("R"))=("R")</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="40" priority="17" operator="beginsWith" text="Python">
       <formula>LEFT((E2),LEN("Python"))=("Python")</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="55" priority="16" operator="beginsWith" text="R">
-      <formula>LEFT((E2),LEN("R"))=("R")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F17">
-    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="Programming">
-      <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
+    <cfRule type="containsText" dxfId="39" priority="3" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="3" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(E2))))</formula>
+    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Exam">
+      <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="5" operator="containsText" text="Exam">
-      <formula>NOT(ISERROR(SEARCH(("Exam"),(E2))))</formula>
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Programming">
+      <formula>NOT(ISERROR(SEARCH(("Programming"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F5 K1 E16:F17">
-    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="35" priority="2" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(K1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14422,111 +14411,115 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="containsText" dxfId="49" priority="13" operator="containsText" text="I">
-      <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
+    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(I2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="11" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(I2))))</formula>
+    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="I">
+      <formula>NOT(ISERROR(SEARCH(("I"),(I2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J1 E5:F5">
-    <cfRule type="containsText" dxfId="46" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J3">
-    <cfRule type="containsText" dxfId="45" priority="72" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="30" priority="72" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4 G4 L4 K4:K7">
-    <cfRule type="containsText" dxfId="44" priority="36" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J7">
-    <cfRule type="containsText" dxfId="43" priority="35" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:J7">
-    <cfRule type="containsText" dxfId="42" priority="199" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="199" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J10">
-    <cfRule type="containsText" dxfId="41" priority="128" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="128" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:J13">
-    <cfRule type="containsText" dxfId="40" priority="212" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="25" priority="212" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J14">
-    <cfRule type="containsText" dxfId="39" priority="205" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="205" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J15">
-    <cfRule type="containsText" dxfId="38" priority="124" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="124" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:J17">
-    <cfRule type="containsText" dxfId="37" priority="68" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="68" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(M30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="36" priority="201" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="21" priority="201" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K10">
-    <cfRule type="containsText" dxfId="35" priority="130" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="20" priority="130" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K13">
-    <cfRule type="containsText" dxfId="34" priority="214" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="19" priority="214" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="33" priority="207" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="18" priority="207" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q34))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="32" priority="126" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="17" priority="126" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K17">
-    <cfRule type="containsText" dxfId="31" priority="70" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="16" priority="70" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2 K2:K3">
-    <cfRule type="containsText" dxfId="30" priority="73" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="15" priority="73" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(Q25))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF7805C-9A25-014E-8DE3-513BC4007718}">
-  <dimension ref="A1:M40"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14536,66 +14529,65 @@
     <col min="3" max="3" width="11.6640625" style="187" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" style="185" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.1640625" style="185" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="185" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="185" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="185"/>
-    <col min="10" max="10" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="185" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.83203125" style="185" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="185"/>
+    <col min="6" max="6" width="13.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="185"/>
+    <col min="9" max="9" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" style="185" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="185"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="185" t="s">
         <v>142</v>
       </c>
       <c r="B1" s="185" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C1" s="187" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="185" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="185" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="185" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="185" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="185" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="185" t="s">
+      <c r="J1" s="185" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="185" t="s">
+      <c r="K1" s="187" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="185" t="s">
-        <v>166</v>
-      </c>
-      <c r="H1" s="185" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="185" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" s="185" t="s">
-        <v>176</v>
-      </c>
-      <c r="L1" s="187" t="s">
-        <v>177</v>
-      </c>
-      <c r="M1" s="185" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J2" s="185">
+      <c r="L1" s="185" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="185">
         <v>5</v>
       </c>
-      <c r="K2" s="187">
+      <c r="J2" s="187">
         <v>0.5</v>
       </c>
-      <c r="L2" s="185" t="s">
+      <c r="K2" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="190" t="s">
+      <c r="L2" s="190" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="185" t="s">
         <v>141</v>
       </c>
@@ -14611,37 +14603,37 @@
       <c r="E3" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="J3" s="185">
+      <c r="F3" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="185">
         <v>11</v>
       </c>
-      <c r="K3" s="187">
+      <c r="J3" s="187">
         <v>0.45</v>
       </c>
-      <c r="L3" s="185" t="s">
+      <c r="K3" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="190" t="s">
+      <c r="L3" s="190" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J4" s="185">
+    <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="185">
         <v>4</v>
       </c>
-      <c r="K4" s="187">
+      <c r="J4" s="187">
         <v>0.4</v>
       </c>
-      <c r="L4" s="185" t="s">
+      <c r="K4" s="185" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="190" t="s">
+      <c r="L4" s="190" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="185" t="s">
         <v>140</v>
       </c>
@@ -14657,26 +14649,26 @@
       <c r="E5" s="189" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="H5" s="185">
+      <c r="F5" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="185">
         <v>34</v>
       </c>
-      <c r="J5" s="185">
+      <c r="I5" s="185">
         <v>9</v>
       </c>
-      <c r="K5" s="187">
+      <c r="J5" s="187">
         <v>0.33</v>
       </c>
-      <c r="L5" s="185" t="s">
+      <c r="K5" s="185" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="190" t="s">
+      <c r="L5" s="190" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="188" t="s">
         <v>16</v>
       </c>
@@ -14689,40 +14681,40 @@
       <c r="E6" s="189" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="H6" s="185">
+      <c r="F6" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="185">
         <v>38</v>
       </c>
-      <c r="J6" s="185">
+      <c r="I6" s="185">
         <v>13</v>
       </c>
-      <c r="K6" s="187">
+      <c r="J6" s="187">
         <v>0.31</v>
       </c>
-      <c r="L6" s="185" t="s">
+      <c r="K6" s="185" t="s">
         <v>118</v>
       </c>
-      <c r="M6" s="191" t="s">
+      <c r="L6" s="191" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J7" s="185">
+    <row r="7" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="185">
         <v>10</v>
       </c>
-      <c r="K7" s="187">
+      <c r="J7" s="187">
         <v>0.3</v>
       </c>
-      <c r="L7" s="185" t="s">
+      <c r="K7" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="190" t="s">
+      <c r="L7" s="190" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="185" t="s">
         <v>143</v>
       </c>
@@ -14739,25 +14731,22 @@
         <v>39</v>
       </c>
       <c r="F8" s="185" t="s">
-        <v>153</v>
-      </c>
-      <c r="G8" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="J8" s="185">
+        <v>154</v>
+      </c>
+      <c r="I8" s="185">
         <v>12</v>
       </c>
-      <c r="K8" s="187">
+      <c r="J8" s="187">
         <v>0.3</v>
       </c>
-      <c r="L8" s="185" t="s">
+      <c r="K8" s="185" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="190" t="s">
+      <c r="L8" s="190" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="188" t="s">
         <v>16</v>
       </c>
@@ -14770,101 +14759,98 @@
       <c r="E9" s="189" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="J9" s="185">
+      <c r="F9" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="185">
         <v>6</v>
       </c>
-      <c r="K9" s="187">
+      <c r="J9" s="187">
         <v>0.3</v>
       </c>
-      <c r="L9" s="185" t="s">
+      <c r="K9" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="M9" s="190" t="s">
+      <c r="L9" s="190" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J10" s="185">
+    <row r="10" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="185">
         <v>3</v>
       </c>
-      <c r="K10" s="187">
+      <c r="J10" s="187">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L10" s="185" t="s">
+      <c r="K10" s="185" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="190" t="s">
+      <c r="L10" s="190" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="185" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="185" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="187">
+      <c r="B11" s="188" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="192">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D11" s="185" t="s">
+      <c r="D11" s="188" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="190" t="s">
+      <c r="E11" s="189" t="s">
         <v>45</v>
       </c>
       <c r="F11" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="J11" s="185">
+      <c r="I11" s="185">
         <v>7</v>
       </c>
-      <c r="K11" s="187">
+      <c r="J11" s="187">
         <v>0.25</v>
       </c>
-      <c r="L11" s="185" t="s">
+      <c r="K11" s="185" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="190" t="s">
+      <c r="L11" s="190" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="185" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="187">
+    <row r="12" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="188" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="192">
         <v>0.4</v>
       </c>
-      <c r="D12" s="185" t="s">
+      <c r="D12" s="188" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="190" t="s">
+      <c r="E12" s="189" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="J12" s="185">
+      <c r="F12" s="185" t="s">
+        <v>154</v>
+      </c>
+      <c r="I12" s="185">
         <v>8</v>
       </c>
-      <c r="K12" s="187">
+      <c r="J12" s="187">
         <v>0.22</v>
       </c>
-      <c r="L12" s="185" t="s">
+      <c r="K12" s="185" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="190" t="s">
+      <c r="L12" s="190" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="185" t="s">
         <v>145</v>
       </c>
@@ -14881,15 +14867,12 @@
         <v>25</v>
       </c>
       <c r="F14" s="185" t="s">
-        <v>155</v>
-      </c>
-      <c r="G14" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C15" s="193">
         <v>0.2</v>
@@ -14901,18 +14884,15 @@
         <v>82</v>
       </c>
       <c r="F15" s="185" t="s">
-        <v>156</v>
-      </c>
-      <c r="G15" s="185" t="s">
-        <v>158</v>
-      </c>
-      <c r="J15" s="185" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="I15" s="185" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C16" s="187">
         <v>0.5</v>
@@ -14923,16 +14903,16 @@
       <c r="E16" s="190" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="185" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="185" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="185" t="s">
         <v>146</v>
       </c>
       <c r="B18" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C18" s="187">
         <v>0.3</v>
@@ -14944,13 +14924,10 @@
         <v>87</v>
       </c>
       <c r="F18" s="185" t="s">
-        <v>157</v>
-      </c>
-      <c r="G18" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="185" t="s">
         <v>28</v>
       </c>
@@ -14963,11 +14940,11 @@
       <c r="E19" s="196" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="185" t="s">
         <v>28</v>
       </c>
@@ -14980,21 +14957,21 @@
       <c r="E20" s="190" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="185" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="185" t="s">
         <v>147</v>
       </c>
       <c r="B22" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C22" s="187">
         <v>0.33</v>
@@ -15005,13 +14982,13 @@
       <c r="E22" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C23" s="187">
         <v>0.3</v>
@@ -15022,13 +14999,13 @@
       <c r="E23" s="190" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C24" s="187">
         <v>0.45</v>
@@ -15039,11 +15016,11 @@
       <c r="E24" s="190" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="185" t="s">
         <v>149</v>
       </c>
@@ -15059,11 +15036,11 @@
       <c r="E26" s="196" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="185" t="s">
         <v>28</v>
       </c>
@@ -15076,13 +15053,13 @@
       <c r="E27" s="196" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="185" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C28" s="193">
         <v>0.1</v>
@@ -15093,11 +15070,11 @@
       <c r="E28" s="196" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F28" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="185" t="s">
         <v>150</v>
       </c>
@@ -15113,11 +15090,11 @@
       <c r="E30" s="197" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="185" t="s">
         <v>28</v>
       </c>
@@ -15130,11 +15107,11 @@
       <c r="E31" s="196" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="185" t="s">
         <v>28</v>
       </c>
@@ -15147,16 +15124,16 @@
       <c r="E32" s="196" t="s">
         <v>63</v>
       </c>
-      <c r="G32" s="185" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="185" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="185" t="s">
         <v>151</v>
       </c>
       <c r="B34" s="185" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C34" s="187">
         <v>0.3</v>
@@ -15167,13 +15144,13 @@
       <c r="E34" s="190" t="s">
         <v>90</v>
       </c>
-      <c r="G34" s="185" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F34" s="185" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C35" s="193">
         <v>0.2</v>
@@ -15184,13 +15161,13 @@
       <c r="E35" s="195" t="s">
         <v>125</v>
       </c>
-      <c r="G35" s="185" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F35" s="185" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C36" s="193">
         <v>0.2</v>
@@ -15201,13 +15178,13 @@
       <c r="E36" s="195" t="s">
         <v>127</v>
       </c>
-      <c r="G36" s="185" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="185" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C37" s="193">
         <v>0.2</v>
@@ -15218,11 +15195,11 @@
       <c r="E37" s="195" t="s">
         <v>129</v>
       </c>
-      <c r="G37" s="185" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F37" s="185" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="185" t="s">
         <v>152</v>
       </c>
@@ -15238,11 +15215,11 @@
       <c r="E39" s="191" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="185" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F39" s="185" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="185" t="s">
         <v>28</v>
       </c>
@@ -15255,8 +15232,8 @@
       <c r="E40" s="195" t="s">
         <v>112</v>
       </c>
-      <c r="G40" s="185" t="s">
-        <v>159</v>
+      <c r="F40" s="185" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -15295,12 +15272,13 @@
       <formula>RIGHT((E39),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M12 E8:E9 E14:E16 E18:E20">
+  <conditionalFormatting sqref="L2:L12 E8:E9 E14:E16 E18:E20">
     <cfRule type="endsWith" dxfId="7" priority="20" operator="endsWith" text="*">
       <formula>RIGHT((E2),LEN("*"))=("*")</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -15334,34 +15312,34 @@
         <v>142</v>
       </c>
       <c r="B1" s="199" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C1" s="200" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D1" s="199" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E1" s="199" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G1" s="199" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H1" s="199" t="s">
         <v>137</v>
       </c>
       <c r="J1" s="199" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K1" s="199" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L1" s="200" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="M1" s="199" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15395,7 +15373,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J3" s="185">
         <v>5</v>
@@ -15441,7 +15419,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H5" s="185">
         <v>34</v>
@@ -15473,7 +15451,7 @@
         <v>23</v>
       </c>
       <c r="G6" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H6" s="185">
         <v>38</v>
@@ -15510,7 +15488,7 @@
         <v>143</v>
       </c>
       <c r="B8" s="185" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C8" s="187">
         <v>0.5</v>
@@ -15525,7 +15503,7 @@
         <v>153</v>
       </c>
       <c r="G8" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J8" s="185">
         <v>13</v>
@@ -15554,7 +15532,7 @@
         <v>50</v>
       </c>
       <c r="G9" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J9" s="185">
         <v>10</v>
@@ -15571,7 +15549,7 @@
     </row>
     <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="185" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C10" s="187">
         <v>0.28000000000000003</v>
@@ -15583,7 +15561,7 @@
         <v>45</v>
       </c>
       <c r="G10" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J10" s="185">
         <v>12</v>
@@ -15608,7 +15586,7 @@
         <v>144</v>
       </c>
       <c r="B12" s="185" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C12" s="187">
         <v>0.4</v>
@@ -15646,7 +15624,7 @@
         <v>25</v>
       </c>
       <c r="G13" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J13" s="185">
         <v>3</v>
@@ -15675,7 +15653,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J14" s="185">
         <v>7</v>
@@ -15701,7 +15679,7 @@
         <v>145</v>
       </c>
       <c r="B16" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C16" s="193">
         <v>0.2</v>
@@ -15713,7 +15691,7 @@
         <v>82</v>
       </c>
       <c r="G16" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J16" s="185">
         <v>8</v>
@@ -15742,7 +15720,7 @@
         <v>36</v>
       </c>
       <c r="G17" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15753,7 +15731,7 @@
         <v>146</v>
       </c>
       <c r="B19" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C19" s="187">
         <v>0.5</v>
@@ -15765,12 +15743,12 @@
         <v>84</v>
       </c>
       <c r="G19" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C20" s="187">
         <v>0.3</v>
@@ -15782,7 +15760,7 @@
         <v>87</v>
       </c>
       <c r="G20" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15803,7 +15781,7 @@
         <v>147</v>
       </c>
       <c r="B24" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C24" s="187">
         <v>0.33</v>
@@ -15815,12 +15793,12 @@
         <v>75</v>
       </c>
       <c r="G24" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C25" s="187">
         <v>0.3</v>
@@ -15832,12 +15810,12 @@
         <v>78</v>
       </c>
       <c r="G25" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C26" s="187">
         <v>0.45</v>
@@ -15849,7 +15827,7 @@
         <v>80</v>
       </c>
       <c r="G26" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15869,7 +15847,7 @@
         <v>66</v>
       </c>
       <c r="G28" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15886,12 +15864,12 @@
         <v>70</v>
       </c>
       <c r="G29" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="185" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C30" s="193">
         <v>0.1</v>
@@ -15903,7 +15881,7 @@
         <v>72</v>
       </c>
       <c r="G30" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15923,7 +15901,7 @@
         <v>56</v>
       </c>
       <c r="G32" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15940,7 +15918,7 @@
         <v>60</v>
       </c>
       <c r="G33" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15957,7 +15935,7 @@
         <v>63</v>
       </c>
       <c r="G34" s="185" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -15965,7 +15943,7 @@
         <v>151</v>
       </c>
       <c r="B36" s="185" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C36" s="187">
         <v>0.3</v>
@@ -15977,12 +15955,12 @@
         <v>90</v>
       </c>
       <c r="G36" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C37" s="193">
         <v>0.2</v>
@@ -15994,12 +15972,12 @@
         <v>125</v>
       </c>
       <c r="G37" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C38" s="193">
         <v>0.2</v>
@@ -16011,12 +15989,12 @@
         <v>127</v>
       </c>
       <c r="G38" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="185" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C39" s="193">
         <v>0.2</v>
@@ -16028,7 +16006,7 @@
         <v>129</v>
       </c>
       <c r="G39" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -16048,7 +16026,7 @@
         <v>119</v>
       </c>
       <c r="G41" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -16065,7 +16043,7 @@
         <v>112</v>
       </c>
       <c r="G42" s="185" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -16105,6 +16083,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -16124,10 +16103,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="204" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="206" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B1" s="207" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="204" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.15">
@@ -16135,7 +16114,7 @@
         <v>5303</v>
       </c>
       <c r="B2" s="205" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28" x14ac:dyDescent="0.15">
@@ -16143,10 +16122,11 @@
         <v>5304</v>
       </c>
       <c r="B3" s="205" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update core and resources
</commit_message>
<xml_diff>
--- a/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
+++ b/Resources/University of Colorado Boulder/Final Assignments by Course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantalbot/Desktop/MSDS/Resources/University of Colorado Boulder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC1FC8D-417B-2347-9302-33DE32CC3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB3928B-06CE-C14F-A920-1746E4B574A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="22880" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22880" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="243">
   <si>
     <t>Course Code</t>
   </si>
@@ -766,6 +766,15 @@
   </si>
   <si>
     <t>9 of 9</t>
+  </si>
+  <si>
+    <t>paper diploma will be mailed approx. eight weeks after the end of the session in which you complete your degree requirements</t>
+  </si>
+  <si>
+    <t>students who have met the degree requirements will receive an email confirming their degree conferral about 3-4 weeks after classes end for the session</t>
+  </si>
+  <si>
+    <t>Nov. 7 degree and certificates conferred</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1429,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="341">
+  <cellXfs count="322">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2126,6 +2135,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2137,71 +2166,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="16" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2233,30 +2201,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00FFFF"/>
           <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2423,6 +2367,22 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFF00FF"/>
           <bgColor rgb="FFFF00FF"/>
         </patternFill>
@@ -2489,6 +2449,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFD966"/>
           <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2639,8 +2607,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-          <bgColor rgb="FF00FFFF"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2655,8 +2623,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2679,16 +2647,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2759,6 +2727,38 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF6D9EEB"/>
           <bgColor rgb="FF6D9EEB"/>
         </patternFill>
@@ -2775,8 +2775,72 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFFE599"/>
           <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FFFFE599"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2815,96 +2879,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6D9EEB"/>
-          <bgColor rgb="FF6D9EEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE599"/>
-          <bgColor rgb="FFFFE599"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2913,14 +2889,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFEAD1DC"/>
           <bgColor rgb="FFEAD1DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2983,14 +2951,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD5A6BD"/>
-          <bgColor rgb="FFD5A6BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFFE599"/>
           <bgColor rgb="FFFFE599"/>
         </patternFill>
@@ -3007,8 +2967,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFD5A6BD"/>
+          <bgColor rgb="FFD5A6BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFFD966"/>
           <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3039,14 +3015,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFFD966"/>
           <bgColor rgb="FFFFD966"/>
         </patternFill>
@@ -3071,16 +3039,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3626,17 +3594,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="305"/>
-      <c r="B1" s="306"/>
-      <c r="C1" s="306"/>
-      <c r="D1" s="306"/>
-      <c r="E1" s="306"/>
-      <c r="F1" s="306"/>
-      <c r="G1" s="306"/>
-      <c r="H1" s="306"/>
-      <c r="I1" s="306"/>
-      <c r="J1" s="306"/>
-      <c r="K1" s="306"/>
+      <c r="A1" s="315"/>
+      <c r="B1" s="316"/>
+      <c r="C1" s="316"/>
+      <c r="D1" s="316"/>
+      <c r="E1" s="316"/>
+      <c r="F1" s="316"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="316"/>
+      <c r="I1" s="316"/>
+      <c r="J1" s="316"/>
+      <c r="K1" s="316"/>
     </row>
     <row r="2" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -4843,15 +4811,15 @@
         <v>88</v>
       </c>
       <c r="D35" s="52"/>
-      <c r="E35" s="307" t="s">
+      <c r="E35" s="317" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="306"/>
-      <c r="G35" s="306"/>
-      <c r="H35" s="306"/>
-      <c r="I35" s="306"/>
-      <c r="J35" s="306"/>
-      <c r="K35" s="306"/>
+      <c r="F35" s="316"/>
+      <c r="G35" s="316"/>
+      <c r="H35" s="316"/>
+      <c r="I35" s="316"/>
+      <c r="J35" s="316"/>
+      <c r="K35" s="316"/>
     </row>
     <row r="36" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38" t="s">
@@ -4864,15 +4832,15 @@
         <v>88</v>
       </c>
       <c r="D36" s="53"/>
-      <c r="E36" s="307" t="s">
+      <c r="E36" s="317" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="306"/>
-      <c r="G36" s="306"/>
-      <c r="H36" s="306"/>
-      <c r="I36" s="306"/>
-      <c r="J36" s="306"/>
-      <c r="K36" s="306"/>
+      <c r="F36" s="316"/>
+      <c r="G36" s="316"/>
+      <c r="H36" s="316"/>
+      <c r="I36" s="316"/>
+      <c r="J36" s="316"/>
+      <c r="K36" s="316"/>
     </row>
     <row r="37" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
@@ -4918,15 +4886,15 @@
         <v>88</v>
       </c>
       <c r="D38" s="52"/>
-      <c r="E38" s="307" t="s">
+      <c r="E38" s="317" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="306"/>
-      <c r="G38" s="306"/>
-      <c r="H38" s="306"/>
-      <c r="I38" s="306"/>
-      <c r="J38" s="306"/>
-      <c r="K38" s="306"/>
+      <c r="F38" s="316"/>
+      <c r="G38" s="316"/>
+      <c r="H38" s="316"/>
+      <c r="I38" s="316"/>
+      <c r="J38" s="316"/>
+      <c r="K38" s="316"/>
     </row>
     <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -4939,15 +4907,15 @@
         <v>88</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="308" t="s">
+      <c r="E39" s="318" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="309"/>
-      <c r="G39" s="309"/>
-      <c r="H39" s="309"/>
-      <c r="I39" s="309"/>
-      <c r="J39" s="309"/>
-      <c r="K39" s="309"/>
+      <c r="F39" s="319"/>
+      <c r="G39" s="319"/>
+      <c r="H39" s="319"/>
+      <c r="I39" s="319"/>
+      <c r="J39" s="319"/>
+      <c r="K39" s="319"/>
     </row>
     <row r="40" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="63" t="s">
@@ -13801,7 +13769,7 @@
   <customSheetViews>
     <customSheetView guid="{41F2DEF0-0911-45DF-AB18-151E8967207B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:K42" xr:uid="{48AB3479-D303-7942-A8F7-09F4978ADD16}">
+      <autoFilter ref="A2:K42" xr:uid="{C6E8EF84-B778-7443-BBC1-FB6220310CC5}">
         <filterColumn colId="2">
           <filters>
             <filter val="Elective"/>
@@ -16747,71 +16715,71 @@
       <c r="M40" s="71"/>
       <c r="N40" s="265"/>
     </row>
-    <row r="41" spans="1:41" s="327" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="336" t="s">
+    <row r="41" spans="1:41" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="168" t="s">
         <v>229</v>
       </c>
       <c r="B41" s="201" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="334">
+      <c r="C41" s="312">
         <v>100</v>
       </c>
-      <c r="D41" s="333" t="s">
+      <c r="D41" s="311" t="s">
         <v>232</v>
       </c>
-      <c r="E41" s="323" t="s">
+      <c r="E41" s="157" t="s">
         <v>233</v>
       </c>
       <c r="F41" s="157" t="s">
         <v>88</v>
       </c>
-      <c r="G41" s="324"/>
+      <c r="G41" s="8"/>
       <c r="H41" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="325"/>
-      <c r="J41" s="326"/>
-      <c r="K41" s="323"/>
+      <c r="I41" s="255"/>
+      <c r="J41" s="158"/>
+      <c r="K41" s="157"/>
       <c r="L41" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="M41" s="324"/>
-      <c r="N41" s="323"/>
-    </row>
-    <row r="42" spans="1:41" s="332" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="340" t="s">
+      <c r="M41" s="8"/>
+      <c r="N41" s="157"/>
+    </row>
+    <row r="42" spans="1:41" s="185" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="183" t="s">
         <v>229</v>
       </c>
       <c r="B42" s="206" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="335">
+      <c r="C42" s="313">
         <v>100</v>
       </c>
       <c r="D42" s="258" t="s">
         <v>234</v>
       </c>
-      <c r="E42" s="328" t="s">
+      <c r="E42" s="180" t="s">
         <v>235</v>
       </c>
       <c r="F42" s="189" t="s">
         <v>88</v>
       </c>
-      <c r="G42" s="329"/>
+      <c r="G42" s="100"/>
       <c r="H42" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="I42" s="330" t="s">
+      <c r="I42" s="259" t="s">
         <v>236</v>
       </c>
-      <c r="J42" s="331"/>
-      <c r="K42" s="328"/>
+      <c r="J42" s="260"/>
+      <c r="K42" s="180"/>
       <c r="L42" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="M42" s="329"/>
-      <c r="N42" s="328"/>
+      <c r="M42" s="100"/>
+      <c r="N42" s="180"/>
     </row>
     <row r="43" spans="1:41" s="277" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="291">
@@ -17063,11 +17031,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F44">
-    <cfRule type="containsText" dxfId="108" priority="124" operator="containsText" text="pathway">
+    <cfRule type="containsText" dxfId="108" priority="125" operator="containsText" text="Core">
+      <formula>NOT(ISERROR(SEARCH(("Core"),(F2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="124" operator="containsText" text="pathway">
       <formula>NOT(ISERROR(SEARCH(("pathway"),(F2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="125" operator="containsText" text="Core">
-      <formula>NOT(ISERROR(SEARCH(("Core"),(F2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G13 G23:G24 G33:G39">
@@ -17086,19 +17054,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:G16">
-    <cfRule type="beginsWith" dxfId="103" priority="73" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="103" priority="74" operator="beginsWith" text="Python">
+      <formula>LEFT((G14),LEN("Python"))=("Python")</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="102" priority="73" operator="beginsWith" text="R">
       <formula>LEFT((G14),LEN("R"))=("R")</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="102" priority="74" operator="beginsWith" text="Python">
-      <formula>LEFT((G14),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:G18">
-    <cfRule type="beginsWith" dxfId="101" priority="56" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="101" priority="57" operator="beginsWith" text="Python">
+      <formula>LEFT((G17),LEN("Python"))=("Python")</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="100" priority="56" operator="beginsWith" text="R">
       <formula>LEFT((G17),LEN("R"))=("R")</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="57" operator="beginsWith" text="Python">
-      <formula>LEFT((G17),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27:G29">
@@ -17107,14 +17075,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27:G30">
-    <cfRule type="containsText" dxfId="98" priority="34" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="98" priority="36" operator="containsText" text="Exam">
+      <formula>NOT(ISERROR(SEARCH(("Exam"),(G27))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="34" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(G27))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="35" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="96" priority="35" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(G27))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="36" operator="containsText" text="Exam">
-      <formula>NOT(ISERROR(SEARCH(("Exam"),(G27))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="95" priority="37" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(G27))))</formula>
@@ -17145,25 +17113,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:G43">
-    <cfRule type="beginsWith" dxfId="88" priority="13" operator="beginsWith" text="R">
+    <cfRule type="beginsWith" dxfId="88" priority="14" operator="beginsWith" text="Python">
+      <formula>LEFT((G40),LEN("Python"))=("Python")</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="87" priority="13" operator="beginsWith" text="R">
       <formula>LEFT((G40),LEN("R"))=("R")</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="87" priority="14" operator="beginsWith" text="Python">
-      <formula>LEFT((G40),LEN("Python"))=("Python")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H13">
-    <cfRule type="containsText" dxfId="86" priority="136" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(G2))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="137" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="86" priority="137" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(G2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="138" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="85" priority="138" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(G2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="139" operator="containsText" text="Programming">
+    <cfRule type="containsText" dxfId="84" priority="139" operator="containsText" text="Programming">
       <formula>NOT(ISERROR(SEARCH(("Programming"),(G2))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="136" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H5 M1">
@@ -17177,28 +17145,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:H16">
-    <cfRule type="containsText" dxfId="80" priority="63" operator="containsText" text="Essay">
-      <formula>NOT(ISERROR(SEARCH(("Essay"),(G14))))</formula>
+    <cfRule type="containsText" dxfId="80" priority="66" operator="containsText" text="Programming">
+      <formula>NOT(ISERROR(SEARCH(("Programming"),(G14))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="64" operator="containsText" text="Project">
+    <cfRule type="containsText" dxfId="79" priority="65" operator="containsText" text="Exam">
+      <formula>NOT(ISERROR(SEARCH(("Exam"),(G14))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="64" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(G14))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="65" operator="containsText" text="Exam">
-      <formula>NOT(ISERROR(SEARCH(("Exam"),(G14))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="66" operator="containsText" text="Programming">
-      <formula>NOT(ISERROR(SEARCH(("Programming"),(G14))))</formula>
+    <cfRule type="containsText" dxfId="77" priority="63" operator="containsText" text="Essay">
+      <formula>NOT(ISERROR(SEARCH(("Essay"),(G14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:H18">
-    <cfRule type="containsText" dxfId="76" priority="50" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(M17))))</formula>
+    <cfRule type="containsText" dxfId="76" priority="52" operator="containsText" text="Project">
+      <formula>NOT(ISERROR(SEARCH(("Project"),(G17))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="75" priority="51" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(G17))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="52" operator="containsText" text="Project">
-      <formula>NOT(ISERROR(SEARCH(("Project"),(G17))))</formula>
+    <cfRule type="containsText" dxfId="74" priority="50" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(M17))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="73" priority="53" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(G17))))</formula>
@@ -17208,17 +17176,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:H24 H26:H32">
-    <cfRule type="containsText" dxfId="71" priority="42" operator="containsText" text="Essay">
+    <cfRule type="containsText" dxfId="71" priority="43" operator="containsText" text="Project">
+      <formula>NOT(ISERROR(SEARCH(("Project"),(G23))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="42" operator="containsText" text="Essay">
       <formula>NOT(ISERROR(SEARCH(("Essay"),(G23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="43" operator="containsText" text="Project">
-      <formula>NOT(ISERROR(SEARCH(("Project"),(G23))))</formula>
+    <cfRule type="containsText" dxfId="69" priority="45" operator="containsText" text="Programming">
+      <formula>NOT(ISERROR(SEARCH(("Programming"),(G23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="44" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="68" priority="44" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(G23))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="45" operator="containsText" text="Programming">
-      <formula>NOT(ISERROR(SEARCH(("Programming"),(G23))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:H43">
@@ -17250,11 +17218,11 @@
     <cfRule type="containsText" dxfId="60" priority="18" operator="containsText" text="Project">
       <formula>NOT(ISERROR(SEARCH(("Project"),(H19))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="19" operator="containsText" text="Exam">
+    <cfRule type="containsText" dxfId="59" priority="20" operator="containsText" text="Programming">
+      <formula>NOT(ISERROR(SEARCH(("Programming"),(H19))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="19" operator="containsText" text="Exam">
       <formula>NOT(ISERROR(SEARCH(("Exam"),(H19))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="20" operator="containsText" text="Programming">
-      <formula>NOT(ISERROR(SEARCH(("Programming"),(H19))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H28">
@@ -17376,14 +17344,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K16 K23:K26">
-    <cfRule type="containsText" dxfId="55" priority="69" operator="containsText" text="A">
-      <formula>NOT(ISERROR(SEARCH(("A"),(K2))))</formula>
+    <cfRule type="containsText" dxfId="55" priority="71" operator="containsText" text="I">
+      <formula>NOT(ISERROR(SEARCH(("I"),(K2))))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="54" priority="70" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(K2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="71" operator="containsText" text="I">
-      <formula>NOT(ISERROR(SEARCH(("I"),(K2))))</formula>
+    <cfRule type="containsText" dxfId="53" priority="69" operator="containsText" text="A">
+      <formula>NOT(ISERROR(SEARCH(("A"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14 K15:L17 K23:L24">
@@ -17473,11 +17441,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="containsText" dxfId="34" priority="104" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="34" priority="105" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="104" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="105" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28:L29">
@@ -17486,11 +17454,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="containsText" dxfId="31" priority="101" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="31" priority="102" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="101" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="102" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31:L32">
@@ -17499,11 +17467,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33">
-    <cfRule type="containsText" dxfId="28" priority="98" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="28" priority="99" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="98" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="99" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34:L36">
@@ -17516,112 +17484,112 @@
       <formula>NOT(ISERROR(SEARCH(("Yes"),(P91))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L41">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="1 submission">
+      <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L42">
+    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH(("Yes"),(P97))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L43">
-    <cfRule type="containsText" dxfId="24" priority="539" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="539" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(P92))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="containsText" dxfId="23" priority="534" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="20" priority="534" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S51))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M8">
-    <cfRule type="containsText" dxfId="22" priority="509" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="19" priority="509" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S58))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:M9">
-    <cfRule type="containsText" dxfId="21" priority="499" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="18" priority="499" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="containsText" dxfId="20" priority="516" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="17" priority="516" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S61))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:M12">
-    <cfRule type="containsText" dxfId="19" priority="371" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="16" priority="371" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S52))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="containsText" dxfId="18" priority="528" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="15" priority="528" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S57))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="containsText" dxfId="17" priority="40" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="14" priority="40" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="16" priority="562" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="13" priority="562" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="containsText" dxfId="15" priority="588" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="12" priority="588" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S30))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="containsText" dxfId="14" priority="517" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="11" priority="517" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M27:M28">
-    <cfRule type="containsText" dxfId="13" priority="480" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="10" priority="480" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S60))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="containsText" dxfId="12" priority="471" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="9" priority="471" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S61))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30:M31">
-    <cfRule type="containsText" dxfId="11" priority="107" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="8" priority="107" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S75))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32:M36">
-    <cfRule type="containsText" dxfId="10" priority="109" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="7" priority="109" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S50))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M37:M38">
-    <cfRule type="containsText" dxfId="9" priority="540" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="6" priority="540" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S54))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M39:M42">
-    <cfRule type="containsText" dxfId="8" priority="542" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="5" priority="542" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S54))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43">
-    <cfRule type="containsText" dxfId="7" priority="537" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="4" priority="537" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(S55))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:N2">
-    <cfRule type="containsText" dxfId="6" priority="532" operator="containsText" text="1 submission">
+    <cfRule type="containsText" dxfId="3" priority="532" operator="containsText" text="1 submission">
       <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L41">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="1 submission">
-      <formula>NOT(ISERROR(SEARCH(("1 submission"),(#REF!))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(#REF!))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L42">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH(("Yes"),(P97))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17636,8 +17604,8 @@
   </sheetPr>
   <dimension ref="A1:AB74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17657,81 +17625,61 @@
     <col min="13" max="16384" width="10.83203125" style="167"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="312" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="312" t="s">
+    <row r="1" spans="1:28" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="306" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="312" t="s">
+      <c r="B1" s="306" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="313" t="s">
+      <c r="C1" s="307" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="312" t="s">
+      <c r="D1" s="306" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="312" t="s">
+      <c r="E1" s="306" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="312" t="s">
+      <c r="F1" s="306" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="312" t="s">
+      <c r="G1" s="306" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="318"/>
-      <c r="I1" s="318"/>
-      <c r="J1" s="318"/>
-      <c r="K1" s="319"/>
-      <c r="L1" s="318"/>
-      <c r="M1" s="318"/>
-      <c r="N1" s="318"/>
-      <c r="O1" s="318"/>
-      <c r="P1" s="318"/>
-      <c r="Q1" s="318"/>
-      <c r="R1" s="318"/>
-      <c r="S1" s="318"/>
-      <c r="T1" s="318"/>
-      <c r="U1" s="318"/>
-      <c r="V1" s="318"/>
-      <c r="W1" s="318"/>
-      <c r="X1" s="318"/>
-      <c r="Y1" s="318"/>
-      <c r="Z1" s="318"/>
-      <c r="AA1" s="318"/>
-      <c r="AB1" s="318"/>
-    </row>
-    <row r="2" spans="1:28" s="315" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="314" t="s">
+      <c r="K1" s="310"/>
+    </row>
+    <row r="2" spans="1:28" s="308" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="321" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="314"/>
-      <c r="C2" s="314"/>
-      <c r="D2" s="314"/>
-      <c r="E2" s="314"/>
-      <c r="F2" s="314"/>
-      <c r="G2" s="314"/>
-      <c r="H2" s="320"/>
-      <c r="I2" s="320"/>
-      <c r="J2" s="320"/>
-      <c r="K2" s="320"/>
-      <c r="L2" s="320"/>
-      <c r="M2" s="320"/>
-      <c r="N2" s="320"/>
-      <c r="O2" s="320"/>
-      <c r="P2" s="320"/>
-      <c r="Q2" s="320"/>
-      <c r="R2" s="320"/>
-      <c r="S2" s="320"/>
-      <c r="T2" s="320"/>
-      <c r="U2" s="320"/>
-      <c r="V2" s="320"/>
-      <c r="W2" s="320"/>
-      <c r="X2" s="320"/>
-      <c r="Y2" s="320"/>
-      <c r="Z2" s="320"/>
-      <c r="AA2" s="320"/>
-      <c r="AB2" s="320"/>
+      <c r="B2" s="321"/>
+      <c r="C2" s="321"/>
+      <c r="D2" s="321"/>
+      <c r="E2" s="321"/>
+      <c r="F2" s="321"/>
+      <c r="G2" s="321"/>
+      <c r="H2" s="309"/>
+      <c r="I2" s="309"/>
+      <c r="J2" s="309"/>
+      <c r="K2" s="309"/>
+      <c r="L2" s="309"/>
+      <c r="M2" s="309"/>
+      <c r="N2" s="309"/>
+      <c r="O2" s="309"/>
+      <c r="P2" s="309"/>
+      <c r="Q2" s="309"/>
+      <c r="R2" s="309"/>
+      <c r="S2" s="309"/>
+      <c r="T2" s="309"/>
+      <c r="U2" s="309"/>
+      <c r="V2" s="309"/>
+      <c r="W2" s="309"/>
+      <c r="X2" s="309"/>
+      <c r="Y2" s="309"/>
+      <c r="Z2" s="309"/>
+      <c r="AA2" s="309"/>
+      <c r="AB2" s="309"/>
     </row>
     <row r="3" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="170" t="s">
@@ -17755,51 +17703,13 @@
       <c r="G3" s="246">
         <v>4</v>
       </c>
-      <c r="H3" s="310"/>
-      <c r="I3" s="310"/>
       <c r="J3" s="175"/>
-      <c r="K3" s="310"/>
-      <c r="L3" s="321"/>
-      <c r="M3" s="310"/>
-      <c r="N3" s="310"/>
-      <c r="O3" s="310"/>
-      <c r="P3" s="310"/>
-      <c r="Q3" s="310"/>
-      <c r="R3" s="310"/>
-      <c r="S3" s="310"/>
-      <c r="T3" s="310"/>
-      <c r="U3" s="310"/>
-      <c r="V3" s="310"/>
-      <c r="W3" s="310"/>
-      <c r="X3" s="310"/>
-      <c r="Y3" s="310"/>
-      <c r="Z3" s="310"/>
-      <c r="AA3" s="310"/>
-      <c r="AB3" s="310"/>
+      <c r="L3" s="172"/>
     </row>
     <row r="4" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="170"/>
-      <c r="H4" s="310"/>
-      <c r="I4" s="310"/>
       <c r="J4" s="175"/>
-      <c r="K4" s="310"/>
-      <c r="L4" s="321"/>
-      <c r="M4" s="310"/>
-      <c r="N4" s="310"/>
-      <c r="O4" s="310"/>
-      <c r="P4" s="310"/>
-      <c r="Q4" s="310"/>
-      <c r="R4" s="310"/>
-      <c r="S4" s="310"/>
-      <c r="T4" s="310"/>
-      <c r="U4" s="310"/>
-      <c r="V4" s="310"/>
-      <c r="W4" s="310"/>
-      <c r="X4" s="310"/>
-      <c r="Y4" s="310"/>
-      <c r="Z4" s="310"/>
-      <c r="AA4" s="310"/>
-      <c r="AB4" s="310"/>
+      <c r="L4" s="172"/>
     </row>
     <row r="5" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="170" t="s">
@@ -17823,27 +17733,8 @@
       <c r="G5" s="246">
         <v>4</v>
       </c>
-      <c r="H5" s="310"/>
-      <c r="I5" s="310"/>
       <c r="J5" s="175"/>
-      <c r="K5" s="310"/>
-      <c r="L5" s="321"/>
-      <c r="M5" s="310"/>
-      <c r="N5" s="310"/>
-      <c r="O5" s="310"/>
-      <c r="P5" s="310"/>
-      <c r="Q5" s="310"/>
-      <c r="R5" s="310"/>
-      <c r="S5" s="310"/>
-      <c r="T5" s="310"/>
-      <c r="U5" s="310"/>
-      <c r="V5" s="310"/>
-      <c r="W5" s="310"/>
-      <c r="X5" s="310"/>
-      <c r="Y5" s="310"/>
-      <c r="Z5" s="310"/>
-      <c r="AA5" s="310"/>
-      <c r="AB5" s="310"/>
+      <c r="L5" s="172"/>
     </row>
     <row r="6" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="170"/>
@@ -17865,51 +17756,13 @@
       <c r="G6" s="246">
         <v>4</v>
       </c>
-      <c r="H6" s="310"/>
-      <c r="I6" s="310"/>
       <c r="J6" s="175"/>
-      <c r="K6" s="310"/>
-      <c r="L6" s="322"/>
-      <c r="M6" s="310"/>
-      <c r="N6" s="310"/>
-      <c r="O6" s="310"/>
-      <c r="P6" s="310"/>
-      <c r="Q6" s="310"/>
-      <c r="R6" s="310"/>
-      <c r="S6" s="310"/>
-      <c r="T6" s="310"/>
-      <c r="U6" s="310"/>
-      <c r="V6" s="310"/>
-      <c r="W6" s="310"/>
-      <c r="X6" s="310"/>
-      <c r="Y6" s="310"/>
-      <c r="Z6" s="310"/>
-      <c r="AA6" s="310"/>
-      <c r="AB6" s="310"/>
+      <c r="L6" s="173"/>
     </row>
     <row r="7" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="170"/>
-      <c r="H7" s="310"/>
-      <c r="I7" s="310"/>
       <c r="J7" s="175"/>
-      <c r="K7" s="310"/>
-      <c r="L7" s="321"/>
-      <c r="M7" s="310"/>
-      <c r="N7" s="310"/>
-      <c r="O7" s="310"/>
-      <c r="P7" s="310"/>
-      <c r="Q7" s="310"/>
-      <c r="R7" s="310"/>
-      <c r="S7" s="310"/>
-      <c r="T7" s="310"/>
-      <c r="U7" s="310"/>
-      <c r="V7" s="310"/>
-      <c r="W7" s="310"/>
-      <c r="X7" s="310"/>
-      <c r="Y7" s="310"/>
-      <c r="Z7" s="310"/>
-      <c r="AA7" s="310"/>
-      <c r="AB7" s="310"/>
+      <c r="L7" s="172"/>
     </row>
     <row r="8" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="170" t="s">
@@ -17933,27 +17786,8 @@
       <c r="G8" s="246">
         <v>4</v>
       </c>
-      <c r="H8" s="310"/>
-      <c r="I8" s="310"/>
       <c r="J8" s="175"/>
-      <c r="K8" s="310"/>
-      <c r="L8" s="321"/>
-      <c r="M8" s="310"/>
-      <c r="N8" s="310"/>
-      <c r="O8" s="310"/>
-      <c r="P8" s="310"/>
-      <c r="Q8" s="310"/>
-      <c r="R8" s="310"/>
-      <c r="S8" s="310"/>
-      <c r="T8" s="310"/>
-      <c r="U8" s="310"/>
-      <c r="V8" s="310"/>
-      <c r="W8" s="310"/>
-      <c r="X8" s="310"/>
-      <c r="Y8" s="310"/>
-      <c r="Z8" s="310"/>
-      <c r="AA8" s="310"/>
-      <c r="AB8" s="310"/>
+      <c r="L8" s="172"/>
     </row>
     <row r="9" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="170"/>
@@ -17975,51 +17809,13 @@
       <c r="G9" s="246">
         <v>4</v>
       </c>
-      <c r="H9" s="310"/>
-      <c r="I9" s="310"/>
       <c r="J9" s="175"/>
-      <c r="K9" s="310"/>
-      <c r="L9" s="321"/>
-      <c r="M9" s="310"/>
-      <c r="N9" s="310"/>
-      <c r="O9" s="310"/>
-      <c r="P9" s="310"/>
-      <c r="Q9" s="310"/>
-      <c r="R9" s="310"/>
-      <c r="S9" s="310"/>
-      <c r="T9" s="310"/>
-      <c r="U9" s="310"/>
-      <c r="V9" s="310"/>
-      <c r="W9" s="310"/>
-      <c r="X9" s="310"/>
-      <c r="Y9" s="310"/>
-      <c r="Z9" s="310"/>
-      <c r="AA9" s="310"/>
-      <c r="AB9" s="310"/>
+      <c r="L9" s="172"/>
     </row>
     <row r="10" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="170"/>
-      <c r="H10" s="310"/>
-      <c r="I10" s="310"/>
       <c r="J10" s="175"/>
-      <c r="K10" s="310"/>
-      <c r="L10" s="321"/>
-      <c r="M10" s="310"/>
-      <c r="N10" s="310"/>
-      <c r="O10" s="310"/>
-      <c r="P10" s="310"/>
-      <c r="Q10" s="310"/>
-      <c r="R10" s="310"/>
-      <c r="S10" s="310"/>
-      <c r="T10" s="310"/>
-      <c r="U10" s="310"/>
-      <c r="V10" s="310"/>
-      <c r="W10" s="310"/>
-      <c r="X10" s="310"/>
-      <c r="Y10" s="310"/>
-      <c r="Z10" s="310"/>
-      <c r="AA10" s="310"/>
-      <c r="AB10" s="310"/>
+      <c r="L10" s="172"/>
     </row>
     <row r="11" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="170" t="s">
@@ -18043,27 +17839,8 @@
       <c r="G11" s="246">
         <v>4</v>
       </c>
-      <c r="H11" s="310"/>
-      <c r="I11" s="310"/>
       <c r="J11" s="175"/>
-      <c r="K11" s="310"/>
-      <c r="L11" s="321"/>
-      <c r="M11" s="310"/>
-      <c r="N11" s="310"/>
-      <c r="O11" s="310"/>
-      <c r="P11" s="310"/>
-      <c r="Q11" s="310"/>
-      <c r="R11" s="310"/>
-      <c r="S11" s="310"/>
-      <c r="T11" s="310"/>
-      <c r="U11" s="310"/>
-      <c r="V11" s="310"/>
-      <c r="W11" s="310"/>
-      <c r="X11" s="310"/>
-      <c r="Y11" s="310"/>
-      <c r="Z11" s="310"/>
-      <c r="AA11" s="310"/>
-      <c r="AB11" s="310"/>
+      <c r="L11" s="172"/>
     </row>
     <row r="12" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="170"/>
@@ -18085,51 +17862,11 @@
       <c r="G12" s="246">
         <v>4</v>
       </c>
-      <c r="H12" s="310"/>
-      <c r="I12" s="310"/>
       <c r="J12" s="175"/>
-      <c r="K12" s="310"/>
-      <c r="L12" s="321"/>
-      <c r="M12" s="310"/>
-      <c r="N12" s="310"/>
-      <c r="O12" s="310"/>
-      <c r="P12" s="310"/>
-      <c r="Q12" s="310"/>
-      <c r="R12" s="310"/>
-      <c r="S12" s="310"/>
-      <c r="T12" s="310"/>
-      <c r="U12" s="310"/>
-      <c r="V12" s="310"/>
-      <c r="W12" s="310"/>
-      <c r="X12" s="310"/>
-      <c r="Y12" s="310"/>
-      <c r="Z12" s="310"/>
-      <c r="AA12" s="310"/>
-      <c r="AB12" s="310"/>
+      <c r="L12" s="172"/>
     </row>
     <row r="13" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="170"/>
-      <c r="H13" s="310"/>
-      <c r="I13" s="310"/>
-      <c r="J13" s="310"/>
-      <c r="K13" s="310"/>
-      <c r="L13" s="310"/>
-      <c r="M13" s="310"/>
-      <c r="N13" s="310"/>
-      <c r="O13" s="310"/>
-      <c r="P13" s="310"/>
-      <c r="Q13" s="310"/>
-      <c r="R13" s="310"/>
-      <c r="S13" s="310"/>
-      <c r="T13" s="310"/>
-      <c r="U13" s="310"/>
-      <c r="V13" s="310"/>
-      <c r="W13" s="310"/>
-      <c r="X13" s="310"/>
-      <c r="Y13" s="310"/>
-      <c r="Z13" s="310"/>
-      <c r="AA13" s="310"/>
-      <c r="AB13" s="310"/>
     </row>
     <row r="14" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="170" t="s">
@@ -18153,27 +17890,6 @@
       <c r="G14" s="246">
         <v>4</v>
       </c>
-      <c r="H14" s="310"/>
-      <c r="I14" s="310"/>
-      <c r="J14" s="310"/>
-      <c r="K14" s="310"/>
-      <c r="L14" s="310"/>
-      <c r="M14" s="310"/>
-      <c r="N14" s="310"/>
-      <c r="O14" s="310"/>
-      <c r="P14" s="310"/>
-      <c r="Q14" s="310"/>
-      <c r="R14" s="310"/>
-      <c r="S14" s="310"/>
-      <c r="T14" s="310"/>
-      <c r="U14" s="310"/>
-      <c r="V14" s="310"/>
-      <c r="W14" s="310"/>
-      <c r="X14" s="310"/>
-      <c r="Y14" s="310"/>
-      <c r="Z14" s="310"/>
-      <c r="AA14" s="310"/>
-      <c r="AB14" s="310"/>
     </row>
     <row r="15" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="170"/>
@@ -18195,27 +17911,6 @@
       <c r="G15" s="246">
         <v>4</v>
       </c>
-      <c r="H15" s="310"/>
-      <c r="I15" s="310"/>
-      <c r="J15" s="310"/>
-      <c r="K15" s="310"/>
-      <c r="L15" s="310"/>
-      <c r="M15" s="310"/>
-      <c r="N15" s="310"/>
-      <c r="O15" s="310"/>
-      <c r="P15" s="310"/>
-      <c r="Q15" s="310"/>
-      <c r="R15" s="310"/>
-      <c r="S15" s="310"/>
-      <c r="T15" s="310"/>
-      <c r="U15" s="310"/>
-      <c r="V15" s="310"/>
-      <c r="W15" s="310"/>
-      <c r="X15" s="310"/>
-      <c r="Y15" s="310"/>
-      <c r="Z15" s="310"/>
-      <c r="AA15" s="310"/>
-      <c r="AB15" s="310"/>
     </row>
     <row r="16" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="170"/>
@@ -18237,51 +17932,9 @@
       <c r="G16" s="246">
         <v>4</v>
       </c>
-      <c r="H16" s="310"/>
-      <c r="I16" s="310"/>
-      <c r="J16" s="310"/>
-      <c r="K16" s="310"/>
-      <c r="L16" s="310"/>
-      <c r="M16" s="310"/>
-      <c r="N16" s="310"/>
-      <c r="O16" s="310"/>
-      <c r="P16" s="310"/>
-      <c r="Q16" s="310"/>
-      <c r="R16" s="310"/>
-      <c r="S16" s="310"/>
-      <c r="T16" s="310"/>
-      <c r="U16" s="310"/>
-      <c r="V16" s="310"/>
-      <c r="W16" s="310"/>
-      <c r="X16" s="310"/>
-      <c r="Y16" s="310"/>
-      <c r="Z16" s="310"/>
-      <c r="AA16" s="310"/>
-      <c r="AB16" s="310"/>
     </row>
     <row r="17" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="170"/>
-      <c r="H17" s="310"/>
-      <c r="I17" s="310"/>
-      <c r="J17" s="310"/>
-      <c r="K17" s="310"/>
-      <c r="L17" s="310"/>
-      <c r="M17" s="310"/>
-      <c r="N17" s="310"/>
-      <c r="O17" s="310"/>
-      <c r="P17" s="310"/>
-      <c r="Q17" s="310"/>
-      <c r="R17" s="310"/>
-      <c r="S17" s="310"/>
-      <c r="T17" s="310"/>
-      <c r="U17" s="310"/>
-      <c r="V17" s="310"/>
-      <c r="W17" s="310"/>
-      <c r="X17" s="310"/>
-      <c r="Y17" s="310"/>
-      <c r="Z17" s="310"/>
-      <c r="AA17" s="310"/>
-      <c r="AB17" s="310"/>
     </row>
     <row r="18" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="170" t="s">
@@ -18305,27 +17958,6 @@
       <c r="G18" s="246">
         <v>2.7</v>
       </c>
-      <c r="H18" s="310"/>
-      <c r="I18" s="310"/>
-      <c r="J18" s="310"/>
-      <c r="K18" s="310"/>
-      <c r="L18" s="310"/>
-      <c r="M18" s="310"/>
-      <c r="N18" s="310"/>
-      <c r="O18" s="310"/>
-      <c r="P18" s="310"/>
-      <c r="Q18" s="310"/>
-      <c r="R18" s="310"/>
-      <c r="S18" s="310"/>
-      <c r="T18" s="310"/>
-      <c r="U18" s="310"/>
-      <c r="V18" s="310"/>
-      <c r="W18" s="310"/>
-      <c r="X18" s="310"/>
-      <c r="Y18" s="310"/>
-      <c r="Z18" s="310"/>
-      <c r="AA18" s="310"/>
-      <c r="AB18" s="310"/>
     </row>
     <row r="19" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="170"/>
@@ -18347,82 +17979,38 @@
       <c r="G19" s="246">
         <v>3.7</v>
       </c>
-      <c r="H19" s="310"/>
-      <c r="I19" s="310"/>
-      <c r="J19" s="310"/>
-      <c r="K19" s="310"/>
-      <c r="L19" s="310"/>
-      <c r="M19" s="310"/>
-      <c r="N19" s="310"/>
-      <c r="O19" s="310"/>
-      <c r="P19" s="310"/>
-      <c r="Q19" s="310"/>
-      <c r="R19" s="310"/>
-      <c r="S19" s="310"/>
-      <c r="T19" s="310"/>
-      <c r="U19" s="310"/>
-      <c r="V19" s="310"/>
-      <c r="W19" s="310"/>
-      <c r="X19" s="310"/>
-      <c r="Y19" s="310"/>
-      <c r="Z19" s="310"/>
-      <c r="AA19" s="310"/>
-      <c r="AB19" s="310"/>
-    </row>
-    <row r="20" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H20" s="310"/>
-      <c r="I20" s="310"/>
-      <c r="J20" s="310"/>
-      <c r="K20" s="310"/>
-      <c r="L20" s="310"/>
-      <c r="M20" s="310"/>
-      <c r="N20" s="310"/>
-      <c r="O20" s="310"/>
-      <c r="P20" s="310"/>
-      <c r="Q20" s="310"/>
-      <c r="R20" s="310"/>
-      <c r="S20" s="310"/>
-      <c r="T20" s="310"/>
-      <c r="U20" s="310"/>
-      <c r="V20" s="310"/>
-      <c r="W20" s="310"/>
-      <c r="X20" s="310"/>
-      <c r="Y20" s="310"/>
-      <c r="Z20" s="310"/>
-      <c r="AA20" s="310"/>
-      <c r="AB20" s="310"/>
-    </row>
-    <row r="21" spans="1:28" s="315" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="314" t="s">
+    </row>
+    <row r="21" spans="1:28" s="308" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="321" t="s">
         <v>228</v>
       </c>
-      <c r="B21" s="314"/>
-      <c r="C21" s="314"/>
-      <c r="D21" s="314"/>
-      <c r="E21" s="314"/>
-      <c r="F21" s="314"/>
-      <c r="G21" s="314"/>
-      <c r="H21" s="320"/>
-      <c r="I21" s="320"/>
-      <c r="J21" s="320"/>
-      <c r="K21" s="320"/>
-      <c r="L21" s="320"/>
-      <c r="M21" s="320"/>
-      <c r="N21" s="320"/>
-      <c r="O21" s="320"/>
-      <c r="P21" s="320"/>
-      <c r="Q21" s="320"/>
-      <c r="R21" s="320"/>
-      <c r="S21" s="320"/>
-      <c r="T21" s="320"/>
-      <c r="U21" s="320"/>
-      <c r="V21" s="320"/>
-      <c r="W21" s="320"/>
-      <c r="X21" s="320"/>
-      <c r="Y21" s="320"/>
-      <c r="Z21" s="320"/>
-      <c r="AA21" s="320"/>
-      <c r="AB21" s="320"/>
+      <c r="B21" s="321"/>
+      <c r="C21" s="321"/>
+      <c r="D21" s="321"/>
+      <c r="E21" s="321"/>
+      <c r="F21" s="321"/>
+      <c r="G21" s="321"/>
+      <c r="H21" s="309"/>
+      <c r="I21" s="309"/>
+      <c r="J21" s="309"/>
+      <c r="K21" s="309"/>
+      <c r="L21" s="309"/>
+      <c r="M21" s="309"/>
+      <c r="N21" s="309"/>
+      <c r="O21" s="309"/>
+      <c r="P21" s="309"/>
+      <c r="Q21" s="309"/>
+      <c r="R21" s="309"/>
+      <c r="S21" s="309"/>
+      <c r="T21" s="309"/>
+      <c r="U21" s="309"/>
+      <c r="V21" s="309"/>
+      <c r="W21" s="309"/>
+      <c r="X21" s="309"/>
+      <c r="Y21" s="309"/>
+      <c r="Z21" s="309"/>
+      <c r="AA21" s="309"/>
+      <c r="AB21" s="309"/>
     </row>
     <row r="22" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="170" t="s">
@@ -18446,27 +18034,6 @@
       <c r="G22" s="246">
         <v>4</v>
       </c>
-      <c r="H22" s="310"/>
-      <c r="I22" s="310"/>
-      <c r="J22" s="310"/>
-      <c r="K22" s="310"/>
-      <c r="L22" s="310"/>
-      <c r="M22" s="310"/>
-      <c r="N22" s="310"/>
-      <c r="O22" s="310"/>
-      <c r="P22" s="310"/>
-      <c r="Q22" s="310"/>
-      <c r="R22" s="310"/>
-      <c r="S22" s="310"/>
-      <c r="T22" s="310"/>
-      <c r="U22" s="310"/>
-      <c r="V22" s="310"/>
-      <c r="W22" s="310"/>
-      <c r="X22" s="310"/>
-      <c r="Y22" s="310"/>
-      <c r="Z22" s="310"/>
-      <c r="AA22" s="310"/>
-      <c r="AB22" s="310"/>
     </row>
     <row r="23" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="170" t="s">
@@ -18490,27 +18057,6 @@
       <c r="G23" s="246">
         <v>4</v>
       </c>
-      <c r="H23" s="310"/>
-      <c r="I23" s="310"/>
-      <c r="J23" s="310"/>
-      <c r="K23" s="310"/>
-      <c r="L23" s="310"/>
-      <c r="M23" s="310"/>
-      <c r="N23" s="310"/>
-      <c r="O23" s="310"/>
-      <c r="P23" s="310"/>
-      <c r="Q23" s="310"/>
-      <c r="R23" s="310"/>
-      <c r="S23" s="310"/>
-      <c r="T23" s="310"/>
-      <c r="U23" s="310"/>
-      <c r="V23" s="310"/>
-      <c r="W23" s="310"/>
-      <c r="X23" s="310"/>
-      <c r="Y23" s="310"/>
-      <c r="Z23" s="310"/>
-      <c r="AA23" s="310"/>
-      <c r="AB23" s="310"/>
     </row>
     <row r="24" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="170"/>
@@ -18532,53 +18078,11 @@
       <c r="G24" s="246">
         <v>3</v>
       </c>
-      <c r="H24" s="310"/>
-      <c r="I24" s="310"/>
-      <c r="J24" s="310"/>
-      <c r="K24" s="310"/>
-      <c r="L24" s="310"/>
-      <c r="M24" s="310"/>
-      <c r="N24" s="310"/>
-      <c r="O24" s="310"/>
-      <c r="P24" s="310"/>
-      <c r="Q24" s="310"/>
-      <c r="R24" s="310"/>
-      <c r="S24" s="310"/>
-      <c r="T24" s="310"/>
-      <c r="U24" s="310"/>
-      <c r="V24" s="310"/>
-      <c r="W24" s="310"/>
-      <c r="X24" s="310"/>
-      <c r="Y24" s="310"/>
-      <c r="Z24" s="310"/>
-      <c r="AA24" s="310"/>
-      <c r="AB24" s="310"/>
     </row>
     <row r="25" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="170"/>
       <c r="C25" s="175"/>
       <c r="E25" s="172"/>
-      <c r="H25" s="310"/>
-      <c r="I25" s="310"/>
-      <c r="J25" s="310"/>
-      <c r="K25" s="310"/>
-      <c r="L25" s="310"/>
-      <c r="M25" s="310"/>
-      <c r="N25" s="310"/>
-      <c r="O25" s="310"/>
-      <c r="P25" s="310"/>
-      <c r="Q25" s="310"/>
-      <c r="R25" s="310"/>
-      <c r="S25" s="310"/>
-      <c r="T25" s="310"/>
-      <c r="U25" s="310"/>
-      <c r="V25" s="310"/>
-      <c r="W25" s="310"/>
-      <c r="X25" s="310"/>
-      <c r="Y25" s="310"/>
-      <c r="Z25" s="310"/>
-      <c r="AA25" s="310"/>
-      <c r="AB25" s="310"/>
     </row>
     <row r="26" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="170" t="s">
@@ -18602,27 +18106,6 @@
       <c r="G26" s="246">
         <v>3</v>
       </c>
-      <c r="H26" s="310"/>
-      <c r="I26" s="310"/>
-      <c r="J26" s="310"/>
-      <c r="K26" s="310"/>
-      <c r="L26" s="310"/>
-      <c r="M26" s="310"/>
-      <c r="N26" s="310"/>
-      <c r="O26" s="310"/>
-      <c r="P26" s="310"/>
-      <c r="Q26" s="310"/>
-      <c r="R26" s="310"/>
-      <c r="S26" s="310"/>
-      <c r="T26" s="310"/>
-      <c r="U26" s="310"/>
-      <c r="V26" s="310"/>
-      <c r="W26" s="310"/>
-      <c r="X26" s="310"/>
-      <c r="Y26" s="310"/>
-      <c r="Z26" s="310"/>
-      <c r="AA26" s="310"/>
-      <c r="AB26" s="310"/>
     </row>
     <row r="27" spans="1:28" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="170" t="s">
@@ -18738,7 +18221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="304"/>
       <c r="B33" s="170" t="s">
         <v>169</v>
@@ -18759,7 +18242,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="304"/>
       <c r="B34" s="157"/>
       <c r="C34" s="157"/>
@@ -18767,7 +18250,7 @@
       <c r="E34" s="157"/>
       <c r="F34" s="168"/>
     </row>
-    <row r="35" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="170" t="s">
         <v>148</v>
       </c>
@@ -18790,7 +18273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="170" t="s">
         <v>167</v>
       </c>
@@ -18813,33 +18296,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="157"/>
     </row>
-    <row r="38" spans="1:10" s="317" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="316" t="s">
+    <row r="38" spans="1:7" s="309" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="320" t="s">
         <v>230</v>
       </c>
-      <c r="B38" s="316"/>
-      <c r="C38" s="316"/>
-      <c r="D38" s="316"/>
-      <c r="E38" s="316"/>
-      <c r="F38" s="316"/>
-      <c r="G38" s="316"/>
-    </row>
-    <row r="39" spans="1:10" s="157" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="314" t="s">
+      <c r="B38" s="320"/>
+      <c r="C38" s="320"/>
+      <c r="D38" s="320"/>
+      <c r="E38" s="320"/>
+      <c r="F38" s="320"/>
+      <c r="G38" s="320"/>
+    </row>
+    <row r="39" spans="1:7" s="157" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="321" t="s">
         <v>237</v>
       </c>
-      <c r="B40" s="314"/>
-      <c r="C40" s="314"/>
-      <c r="D40" s="314"/>
-      <c r="E40" s="314"/>
-      <c r="F40" s="314"/>
-      <c r="G40" s="314"/>
-    </row>
-    <row r="41" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="321"/>
+      <c r="C40" s="321"/>
+      <c r="D40" s="321"/>
+      <c r="E40" s="321"/>
+      <c r="F40" s="321"/>
+      <c r="G40" s="321"/>
+    </row>
+    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="167" t="s">
         <v>231</v>
       </c>
@@ -18862,7 +18345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="170" t="s">
         <v>16</v>
       </c>
@@ -18882,7 +18365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="170" t="s">
         <v>16</v>
       </c>
@@ -18902,7 +18385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="170" t="s">
         <v>16</v>
       </c>
@@ -18922,7 +18405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="170" t="s">
         <v>16</v>
       </c>
@@ -18942,11 +18425,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="177" t="s">
         <v>156</v>
       </c>
-      <c r="C46" s="311">
+      <c r="C46" s="305">
         <v>0.45</v>
       </c>
       <c r="D46" s="177" t="s">
@@ -18959,17 +18442,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="167"/>
       <c r="G48" s="246">
         <f>SUM(G3:G47)</f>
         <v>111.4</v>
       </c>
-      <c r="H48" s="310"/>
-      <c r="I48" s="310"/>
-      <c r="J48" s="310"/>
-    </row>
-    <row r="49" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C49" s="167"/>
       <c r="F49" s="246" t="s">
         <v>206</v>
@@ -18978,73 +18458,72 @@
         <f>SUM(G48/29)</f>
         <v>3.8413793103448279</v>
       </c>
-      <c r="H49" s="310"/>
-      <c r="I49" s="310"/>
-      <c r="J49" s="310"/>
-    </row>
-    <row r="50" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C50" s="167"/>
       <c r="G50" s="247"/>
-      <c r="H50" s="310"/>
-      <c r="I50" s="310"/>
-      <c r="J50" s="310"/>
-    </row>
-    <row r="51" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" s="167"/>
-    </row>
-    <row r="52" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E51" s="167" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="175"/>
       <c r="G52" s="248"/>
     </row>
-    <row r="53" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" s="175"/>
+      <c r="E53" s="167" t="s">
+        <v>241</v>
+      </c>
       <c r="G53" s="248"/>
     </row>
-    <row r="54" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" s="175"/>
       <c r="H54" s="246"/>
-      <c r="I54" s="338"/>
-      <c r="J54" s="338"/>
-      <c r="K54" s="339"/>
-    </row>
-    <row r="55" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I54" s="246"/>
+      <c r="J54" s="246"/>
+    </row>
+    <row r="55" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H55" s="248"/>
-      <c r="I55" s="338"/>
-      <c r="J55" s="338"/>
-      <c r="K55" s="339"/>
-    </row>
-    <row r="56" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I55" s="246"/>
+      <c r="J55" s="246"/>
+    </row>
+    <row r="56" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E56" s="167" t="s">
+        <v>242</v>
+      </c>
       <c r="H56" s="248"/>
-      <c r="I56" s="338"/>
-      <c r="J56" s="338"/>
-      <c r="K56" s="339"/>
-    </row>
-    <row r="57" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I56" s="246"/>
+      <c r="J56" s="246"/>
+    </row>
+    <row r="57" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H57" s="246"/>
-      <c r="I57" s="338"/>
-      <c r="J57" s="338"/>
-      <c r="K57" s="339"/>
-    </row>
-    <row r="58" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E58" s="337"/>
-    </row>
-    <row r="59" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I57" s="246"/>
+      <c r="J57" s="246"/>
+    </row>
+    <row r="58" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E58" s="314"/>
+    </row>
+    <row r="59" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E59"/>
       <c r="I59" s="248"/>
       <c r="J59" s="248"/>
     </row>
-    <row r="60" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E60" s="157"/>
     </row>
-    <row r="62" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" s="175"/>
       <c r="E62" s="172"/>
     </row>
-    <row r="63" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C63" s="175"/>
       <c r="E63" s="172"/>
     </row>
-    <row r="64" spans="3:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C64" s="175"/>
       <c r="E64" s="172"/>
     </row>

</xml_diff>